<commit_message>
Added IAM and Follow tests.
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="0" yWindow="2580" windowWidth="19635" windowHeight="5385"/>
   </bookViews>
   <sheets>
-    <sheet name="Profile" sheetId="1" r:id="rId1"/>
+    <sheet name="IAM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>GET</t>
   </si>
@@ -49,59 +49,37 @@
     <t>STORE</t>
   </si>
   <si>
-    <t>PUT</t>
-  </si>
-  <si>
-    <t>Retrieve user profile</t>
-  </si>
-  <si>
-    <t>1PPROFILE</t>
-  </si>
-  <si>
-    <t>truid</t>
-  </si>
-  <si>
-    <t>Upate user profile</t>
-  </si>
-  <si>
-    <t>Content-Type=application/json</t>
-  </si>
-  <si>
-    <t>{"interest":["computers","science"]}</t>
-  </si>
-  <si>
-    <t>status=200||firstName=Mohana</t>
-  </si>
-  <si>
     <t>status=200</t>
   </si>
   <si>
     <t>APIPATH</t>
   </si>
   <si>
-    <t>/users/user/a99ba4dc-45be-4ad2-9c9e-22e78584b82b</t>
-  </si>
-  <si>
     <t>S1_TC_T1</t>
   </si>
   <si>
-    <t>S1_TC_T2</t>
-  </si>
-  <si>
     <t>DEPENDENCYTESTS</t>
   </si>
   <si>
+    <t>1PAUTH</t>
+  </si>
+  <si>
+    <t>Test authorize API</t>
+  </si>
+  <si>
+    <t>/authorize</t>
+  </si>
+  <si>
+    <t>?provider=thomsonreuters&amp;backurl=%2Fui%2F%23%2Flogin%2FAUTHTOKEN</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>/users/user/(S1_TC_T1_truid)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -171,7 +149,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -187,6 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -482,26 +461,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="48.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="6" width="23.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.7109375" style="6" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -515,7 +494,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -530,7 +509,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>9</v>
@@ -544,66 +523,32 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="H2" s="5"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="K2" s="1"/>
       <c r="L2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3"/>
-      <c r="H3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
         <v>19</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added configuration and code changes to pass the eureka url and env suffix along with maven commandline arguments.
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>GET</t>
   </si>
@@ -80,6 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -469,18 +470,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.7109375" style="6" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="80.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="6" width="23.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">

</xml_diff>

<commit_message>
Added IAM related FB and LinkedIn Authorize API test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>GET</t>
   </si>
@@ -64,13 +64,31 @@
     <t>1PAUTH</t>
   </si>
   <si>
-    <t>Test authorize API</t>
-  </si>
-  <si>
     <t>/authorize</t>
   </si>
   <si>
     <t>?provider=thomsonreuters&amp;backurl=%2Fui%2F%23%2Flogin%2FAUTHTOKEN</t>
+  </si>
+  <si>
+    <t>Test the authorize API for Redirection to TR ID login page</t>
+  </si>
+  <si>
+    <t>S1_TC_T2</t>
+  </si>
+  <si>
+    <t>S1_TC_T3</t>
+  </si>
+  <si>
+    <t>Test the authorize API for Redirection to Facebook login page</t>
+  </si>
+  <si>
+    <t>Test the authorize API for Redirection to Linked-In login page</t>
+  </si>
+  <si>
+    <t>?provider=facebook&amp;backurl=%2Fui%2F%23%2Flogin%2FAUTHTOKEN</t>
+  </si>
+  <si>
+    <t>?provider=linkedin&amp;backurl=%2Fui%2F%23%2Flogin%2FAUTHTOKEN</t>
   </si>
 </sst>
 </file>
@@ -458,24 +476,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.28515625" style="6" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="80.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.7109375" style="6" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6" style="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -484,7 +502,7 @@
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -518,25 +536,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
+      <c r="B2" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="1"/>
@@ -544,6 +562,60 @@
         <v>11</v>
       </c>
       <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" ht="30">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" ht="30">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Avoid reading the empty rows.
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>GET</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>/auth/bucket/f</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -528,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -773,10 +770,9 @@
       </c>
       <c r="K7"/>
       <c r="L7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="21" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added integration code with Extent reports
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t>GET</t>
   </si>
@@ -70,21 +70,12 @@
     <t>?provider=thomsonreuters&amp;backurl=%2Fui%2F%23%2Flogin%2FAUTHTOKEN</t>
   </si>
   <si>
-    <t>Test the authorize API for Redirection to TR ID login page</t>
-  </si>
-  <si>
     <t>S1_TC_T2</t>
   </si>
   <si>
     <t>S1_TC_T3</t>
   </si>
   <si>
-    <t>Test the authorize API for Redirection to Facebook login page</t>
-  </si>
-  <si>
-    <t>Test the authorize API for Redirection to Linked-In login page</t>
-  </si>
-  <si>
     <t>?provider=facebook&amp;backurl=%2Fui%2F%23%2Flogin%2FAUTHTOKEN</t>
   </si>
   <si>
@@ -97,9 +88,6 @@
     <t>S1_TC_T4</t>
   </si>
   <si>
-    <t>Evict user id</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -121,15 +109,9 @@
     <t>{"truid":"(SYS_USER1)" ,"userStatus":"Deactivate"}</t>
   </si>
   <si>
-    <t>Activate evicted user</t>
-  </si>
-  <si>
     <t>S1_TC_T6</t>
   </si>
   <si>
-    <t>Get evicted user info or bucket information</t>
-  </si>
-  <si>
     <t>status=200||truid=(SYS_USER1)</t>
   </si>
   <si>
@@ -148,20 +130,31 @@
     <t>status=200||records.truid=(SYS_USER1)||records.email=project.neon1@gmail.com||count=1</t>
   </si>
   <si>
-    <t>Get User Mail id by passing truid</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>PASS</t>
+    <t>Verify that user is able to evict a user by passing truid</t>
+  </si>
+  <si>
+    <t>Verify that user is able to activate evicted user by passing truid</t>
+  </si>
+  <si>
+    <t>Verify that get evicted user info or bucket information</t>
+  </si>
+  <si>
+    <t>Verify that user able to get User Mail id by passing truid</t>
+  </si>
+  <si>
+    <t>Verify that to test the authorize API for Redirection to Linked-In login page</t>
+  </si>
+  <si>
+    <t>Verify that to test the authorize API for Redirection to Facebook login page</t>
+  </si>
+  <si>
+    <t>Verify that to test the authorize API for Redirection to TR ID login page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -548,24 +541,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L2:L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="6" width="33.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="79.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="6" width="70.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="6" width="43.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.28515625" style="6" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="79" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="70.28515625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="43.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -611,7 +604,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -623,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>17</v>
@@ -634,16 +627,13 @@
         <v>11</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" ht="30">
+    <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -655,10 +645,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="1"/>
@@ -666,16 +656,13 @@
         <v>11</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" ht="30">
+    <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -687,10 +674,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="1"/>
@@ -698,130 +685,102 @@
         <v>11</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="L4" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="J5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="7" t="s">
+    </row>
+    <row r="6" spans="1:12" ht="30">
+      <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="G5"/>
-      <c r="H5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5"/>
-      <c r="J5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
       <c r="B6" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6"/>
-      <c r="H6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6"/>
-      <c r="J6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6"/>
-      <c r="L6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F7"/>
-      <c r="G7"/>
       <c r="H7"/>
-      <c r="I7"/>
       <c r="J7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F8"/>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H8"/>
-      <c r="I8"/>
       <c r="J8" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8"/>
-      <c r="L8" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new test cases in IAM
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>GET</t>
   </si>
@@ -82,9 +82,6 @@
     <t>{"truid":"(SYS_USER1)" ,"userStatus":"Activate"}</t>
   </si>
   <si>
-    <t>status=200||Success=OK</t>
-  </si>
-  <si>
     <t>{"truid":"(SYS_USER1)" ,"userStatus":"Deactivate"}</t>
   </si>
   <si>
@@ -97,12 +94,6 @@
     <t>/users</t>
   </si>
   <si>
-    <t>?truid=(SYS_USER1)</t>
-  </si>
-  <si>
-    <t>status=200||records.truid=(SYS_USER1)||records.email=project.neon1@gmail.com||count=1</t>
-  </si>
-  <si>
     <t>Verify that user is able to evict a user by passing truid</t>
   </si>
   <si>
@@ -149,6 +140,74 @@
   </si>
   <si>
     <t>OPQA-747</t>
+  </si>
+  <si>
+    <t>Verify that user is able to modify Account attributes</t>
+  </si>
+  <si>
+    <t>/users/prefs/(SYS_USER2)/attributes</t>
+  </si>
+  <si>
+    <t>Content-Type=application/json||X-1P-User=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>{
+  "language": "English",
+  "lastSummaryGenerated": "1449834840000",
+  "marketing_optin": "true",
+  "recommendations": "true",
+  "notifications": "true"
+}</t>
+  </si>
+  <si>
+    <t>status=200||notifications=true</t>
+  </si>
+  <si>
+    <t>/auth/accountsettings</t>
+  </si>
+  <si>
+    <t>Verify that user is able to get account attributes</t>
+  </si>
+  <si>
+    <t>Verify that user is able to modify account settings</t>
+  </si>
+  <si>
+    <t>?truid=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>status=200||records.truid=(SYS_USER2)||records.email=project.neon2@gmail.com||count=1</t>
+  </si>
+  <si>
+    <t>records.email</t>
+  </si>
+  <si>
+    <t>{
+  "truid": "(SYS_USER2)",
+  "loginid": "(OPQA-542_records.email)",
+  "provider": "Oneplatform",
+  "notifications": true,
+  "marketing_optin": true,
+  "language": "English",
+  "recommendations": true
+}</t>
+  </si>
+  <si>
+    <t>OPQA-851</t>
+  </si>
+  <si>
+    <t>OPQA-852</t>
+  </si>
+  <si>
+    <t>OPQA-853</t>
+  </si>
+  <si>
+    <t>Verify that user is able to get account settings</t>
+  </si>
+  <si>
+    <t>OPQA-854</t>
+  </si>
+  <si>
+    <t>status=200||recommendations=true</t>
   </si>
 </sst>
 </file>
@@ -539,25 +598,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.28515625" style="6" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33" style="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="58" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="79" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="70.28515625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="43.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -601,10 +660,10 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -630,10 +689,10 @@
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -659,10 +718,10 @@
     </row>
     <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -688,45 +747,43 @@
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>20</v>
@@ -734,53 +791,160 @@
       <c r="H6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H7"/>
       <c r="J7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="H8"/>
       <c r="J8" s="8" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="K8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="105">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10"/>
+      <c r="J10" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="135">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12"/>
+      <c r="I12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -792,8 +956,12 @@
     <hyperlink ref="A5" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-745"/>
     <hyperlink ref="A6" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-746"/>
     <hyperlink ref="A7" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-747"/>
+    <hyperlink ref="A9" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-851"/>
+    <hyperlink ref="A10" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-852"/>
+    <hyperlink ref="A11" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-853"/>
+    <hyperlink ref="A12" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-854"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new test cases to 1PNOTIFY Changed test cases in to 1PTYPEAHEAD AND 1PAUTH
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t>GET</t>
   </si>
@@ -76,33 +76,9 @@
     <t>X-1P-ZUUL-HOST=http://ec2-54-148-94-143.us-west-2.compute.amazonaws.com:7001/</t>
   </si>
   <si>
-    <t>Content-Type=application/json</t>
-  </si>
-  <si>
-    <t>{"truid":"(SYS_USER1)" ,"userStatus":"Activate"}</t>
-  </si>
-  <si>
-    <t>{"truid":"(SYS_USER1)" ,"userStatus":"Deactivate"}</t>
-  </si>
-  <si>
-    <t>status=200||truid=(SYS_USER1)</t>
-  </si>
-  <si>
-    <t>/auth/bucket/f</t>
-  </si>
-  <si>
     <t>/users</t>
   </si>
   <si>
-    <t>Verify that user is able to evict a user by passing truid</t>
-  </si>
-  <si>
-    <t>Verify that user is able to activate evicted user by passing truid</t>
-  </si>
-  <si>
-    <t>Verify that get evicted user info or bucket information</t>
-  </si>
-  <si>
     <t>Verify that user able to get User Mail id by passing truid</t>
   </si>
   <si>
@@ -115,9 +91,6 @@
     <t>Verify that to test the authorize API for Redirection to TR ID login page</t>
   </si>
   <si>
-    <t>/admin/access</t>
-  </si>
-  <si>
     <t>PUT</t>
   </si>
   <si>
@@ -131,15 +104,6 @@
   </si>
   <si>
     <t>OPQA-541</t>
-  </si>
-  <si>
-    <t>OPQA-745</t>
-  </si>
-  <si>
-    <t>OPQA-746</t>
-  </si>
-  <si>
-    <t>OPQA-747</t>
   </si>
   <si>
     <t>Verify that user is able to modify Account attributes</t>
@@ -598,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L12"/>
+      <selection activeCell="L2" sqref="L2:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -660,10 +624,10 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -689,10 +653,10 @@
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -718,10 +682,10 @@
     </row>
     <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -747,221 +711,149 @@
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="5"/>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5"/>
+      <c r="J5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" ht="30">
+    <row r="6" spans="1:12" ht="105">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="5"/>
+      <c r="J6" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>0</v>
       </c>
+      <c r="F7" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="H7"/>
-      <c r="J7" s="8" t="s">
-        <v>23</v>
+      <c r="J7" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30">
+    <row r="8" spans="1:12" ht="135">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8"/>
-      <c r="J8" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" t="s">
-        <v>52</v>
+      <c r="F8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="105">
+    <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="30">
-      <c r="A10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10"/>
-      <c r="J10" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="135">
-      <c r="A11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="30">
-      <c r="A12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12"/>
-      <c r="I12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-542"/>
+    <hyperlink ref="A5" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-542"/>
     <hyperlink ref="A2" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-539"/>
     <hyperlink ref="A3" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-540"/>
     <hyperlink ref="A4" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-541"/>
-    <hyperlink ref="A5" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-745"/>
-    <hyperlink ref="A6" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-746"/>
-    <hyperlink ref="A7" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-747"/>
-    <hyperlink ref="A9" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-851"/>
-    <hyperlink ref="A10" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-852"/>
-    <hyperlink ref="A11" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-853"/>
-    <hyperlink ref="A12" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-854"/>
+    <hyperlink ref="A6" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-851"/>
+    <hyperlink ref="A7" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-852"/>
+    <hyperlink ref="A8" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-853"/>
+    <hyperlink ref="A9" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-854"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Test cases into 1PAUTH
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
   <si>
     <t>GET</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>?provider=linkedin&amp;backurl=%2Fui%2F%23%2Flogin%2FAUTHTOKEN</t>
-  </si>
-  <si>
-    <t>X-1P-ZUUL-HOST=http://ec2-54-148-94-143.us-west-2.compute.amazonaws.com:7001/</t>
   </si>
   <si>
     <t>/users</t>
@@ -137,9 +134,6 @@
   </si>
   <si>
     <t>?truid=(SYS_USER2)</t>
-  </si>
-  <si>
-    <t>status=200||records.truid=(SYS_USER2)||records.email=project.neon2@gmail.com||count=1</t>
   </si>
   <si>
     <t>records.email</t>
@@ -172,6 +166,63 @@
   </si>
   <si>
     <t>status=200||recommendations=true</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>?subject=Update from Project Neon&amp;emailType=summary&amp;template=summary-email.mustache&amp;html=true</t>
+  </si>
+  <si>
+    <t>{
+  "$-id":"NotificationSummaryEmailEvent",
+  "summary":[
+    {"type":"newFollowers","label":"1 person started following you","count":1},
+    {"type":"peopleLikedYourPosts","label":"1 person liked your posts","count":1}
+  ]
+}</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||Reason=User not found</t>
+  </si>
+  <si>
+    <t>?subject=Update from Project Neon&amp;template=summary-email.mustache&amp;html=true</t>
+  </si>
+  <si>
+    <t>status=403||errorcode=403||Reason=Invalid or Empty parameter</t>
+  </si>
+  <si>
+    <t>status=200||records.truid=(SYS_USER2)||count=1</t>
+  </si>
+  <si>
+    <t>/auth/email/(SYS_USER2)a</t>
+  </si>
+  <si>
+    <t>/auth/email/(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>status=200||recipient=(SYS_USER2)||email=(OPQA-542_records.email)||subject=Update from Project Neon</t>
+  </si>
+  <si>
+    <t>Verify that to send update mails from neon</t>
+  </si>
+  <si>
+    <t>Verify that get error status to send update mails from neon by passing empty data</t>
+  </si>
+  <si>
+    <t>Verify that get error status to send update mails from neon by passing wrong user id</t>
+  </si>
+  <si>
+    <t>OPQA-1615</t>
+  </si>
+  <si>
+    <t>OPQA-1616</t>
+  </si>
+  <si>
+    <t>OPQA-1617</t>
   </si>
 </sst>
 </file>
@@ -562,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L9"/>
+      <selection activeCell="L2" sqref="L2:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -576,9 +627,9 @@
     <col min="4" max="4" width="58" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="79" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="70.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="70.28515625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="43.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -603,7 +654,7 @@
       <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -624,10 +675,10 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -638,10 +689,8 @@
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="5"/>
@@ -653,10 +702,10 @@
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -667,10 +716,8 @@
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H3" s="5"/>
@@ -682,10 +729,10 @@
     </row>
     <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -696,10 +743,8 @@
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H4" s="5"/>
@@ -711,52 +756,53 @@
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G5" t="s">
-        <v>38</v>
+      <c r="G5" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="H5"/>
       <c r="J5" s="8" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="105">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6"/>
+      <c r="H6" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>11</v>
@@ -764,52 +810,54 @@
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>32</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G7"/>
       <c r="H7"/>
       <c r="J7" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="135">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" t="s">
         <v>25</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>11</v>
@@ -817,29 +865,120 @@
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>32</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G9"/>
       <c r="H9"/>
       <c r="I9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J9" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="135">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
         <v>47</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="135">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="135">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed Header from Iam Test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
   <si>
     <t>GET</t>
   </si>
@@ -223,9 +223,6 @@
   </si>
   <si>
     <t>OPQA-1617</t>
-  </si>
-  <si>
-    <t>X-1P-ZUUL-HOST=http://ec2-54-148-94-143.us-west-2.compute.amazonaws.com:7001/</t>
   </si>
 </sst>
 </file>
@@ -692,9 +689,7 @@
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>63</v>
-      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="8" t="s">
         <v>16</v>
       </c>
@@ -721,9 +716,7 @@
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>63</v>
-      </c>
+      <c r="F3" s="7"/>
       <c r="G3" s="8" t="s">
         <v>17</v>
       </c>
@@ -750,9 +743,7 @@
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>63</v>
-      </c>
+      <c r="F4" s="7"/>
       <c r="G4" s="8" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Fixed Failing test cases in to IAM
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t>GET</t>
   </si>
@@ -64,18 +64,12 @@
     <t>/authorize</t>
   </si>
   <si>
-    <t>?provider=thomsonreuters&amp;backurl=%2Fui%2F%23%2Flogin%2FAUTHTOKEN</t>
-  </si>
-  <si>
     <t>?provider=facebook&amp;backurl=%2Fui%2F%23%2Flogin%2FAUTHTOKEN</t>
   </si>
   <si>
     <t>?provider=linkedin&amp;backurl=%2Fui%2F%23%2Flogin%2FAUTHTOKEN</t>
   </si>
   <si>
-    <t>/users</t>
-  </si>
-  <si>
     <t>Verify that user able to get User Mail id by passing truid</t>
   </si>
   <si>
@@ -85,16 +79,10 @@
     <t>Verify that to test the authorize API for Redirection to Facebook login page</t>
   </si>
   <si>
-    <t>Verify that to test the authorize API for Redirection to TR ID login page</t>
-  </si>
-  <si>
     <t>PUT</t>
   </si>
   <si>
     <t>OPQA-542</t>
-  </si>
-  <si>
-    <t>OPQA-539</t>
   </si>
   <si>
     <t>OPQA-540</t>
@@ -121,41 +109,12 @@
 }</t>
   </si>
   <si>
-    <t>status=200||notifications=true</t>
-  </si>
-  <si>
-    <t>/auth/accountsettings</t>
-  </si>
-  <si>
-    <t>Verify that user is able to get account attributes</t>
-  </si>
-  <si>
     <t>Verify that user is able to modify account settings</t>
   </si>
   <si>
-    <t>?truid=(SYS_USER2)</t>
-  </si>
-  <si>
-    <t>records.email</t>
-  </si>
-  <si>
-    <t>{
-  "truid": "(SYS_USER2)",
-  "loginid": "(OPQA-542_records.email)",
-  "provider": "Oneplatform",
-  "notifications": true,
-  "marketing_optin": true,
-  "language": "English",
-  "recommendations": true
-}</t>
-  </si>
-  <si>
     <t>OPQA-851</t>
   </si>
   <si>
-    <t>OPQA-852</t>
-  </si>
-  <si>
     <t>OPQA-853</t>
   </si>
   <si>
@@ -163,9 +122,6 @@
   </si>
   <si>
     <t>OPQA-854</t>
-  </si>
-  <si>
-    <t>status=200||recommendations=true</t>
   </si>
   <si>
     <t>POST</t>
@@ -195,18 +151,12 @@
     <t>status=403||errorcode=403||Reason=Invalid or Empty parameter</t>
   </si>
   <si>
-    <t>status=200||records.truid=(SYS_USER2)||count=1</t>
-  </si>
-  <si>
     <t>/auth/email/(SYS_USER2)a</t>
   </si>
   <si>
     <t>/auth/email/(SYS_USER2)</t>
   </si>
   <si>
-    <t>status=200||recipient=(SYS_USER2)||email=(OPQA-542_records.email)||subject=Update from Project Neon</t>
-  </si>
-  <si>
     <t>Verify that to send update mails from neon</t>
   </si>
   <si>
@@ -223,12 +173,43 @@
   </si>
   <si>
     <t>OPQA-1617</t>
+  </si>
+  <si>
+    <t>/account/auth/settings</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>status=200||userid=(SYS_USER2)||preferredProvider=STEAM</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>status=200||notification=true</t>
+  </si>
+  <si>
+    <t>status=200||recipient=(SYS_USER2)||email=(OPQA-542_email)||subject=Update from Project Neon</t>
+  </si>
+  <si>
+    <t>{
+  "userid": "(SYS_USER2)",
+   "notifications": true
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -613,26 +594,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="58" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="79" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="70.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="70.28515625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="43.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="33.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="58.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="79.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="6" width="70.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="6" width="70.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="6" width="43.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -673,12 +654,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row r="2" spans="1:12" ht="45">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -699,13 +680,16 @@
         <v>11</v>
       </c>
       <c r="K2" s="1"/>
+      <c r="L2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -726,64 +710,77 @@
         <v>11</v>
       </c>
       <c r="K3" s="1"/>
+      <c r="L3" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="45">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="F4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="8"/>
       <c r="H4" s="5"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="1"/>
+      <c r="J4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" ht="30">
+    <row r="5" spans="1:12" ht="105">
       <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5"/>
-      <c r="J5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" t="s">
-        <v>38</v>
+        <v>26</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5"/>
+      <c r="L5" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="105">
+    <row r="6" spans="1:12" ht="60">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>29</v>
@@ -792,207 +789,171 @@
         <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G6"/>
       <c r="H6" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="I6"/>
       <c r="J6" s="5" t="s">
         <v>11</v>
+      </c>
+      <c r="K6"/>
+      <c r="L6" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="G7"/>
       <c r="H7"/>
-      <c r="J7" s="5" t="s">
-        <v>33</v>
+      <c r="I7"/>
+      <c r="J7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7"/>
+      <c r="L7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="135">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8"/>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="H8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" t="s">
-        <v>25</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="I8"/>
       <c r="J8" s="5" t="s">
-        <v>11</v>
+        <v>38</v>
+      </c>
+      <c r="K8"/>
+      <c r="L8" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30">
+    <row r="9" spans="1:12" ht="135">
       <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>45</v>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9"/>
+      <c r="J9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9"/>
+      <c r="L9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="135">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="135">
-      <c r="A11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10"/>
+      <c r="L10" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="135">
-      <c r="A12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-542"/>
-    <hyperlink ref="A2" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-539"/>
-    <hyperlink ref="A3" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-540"/>
-    <hyperlink ref="A4" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-541"/>
-    <hyperlink ref="A6" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-851"/>
-    <hyperlink ref="A7" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-852"/>
-    <hyperlink ref="A8" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-853"/>
-    <hyperlink ref="A9" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-854"/>
+    <hyperlink ref="A2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-540"/>
+    <hyperlink ref="A3" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-541"/>
+    <hyperlink ref="A5" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-851"/>
+    <hyperlink ref="A6" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-853"/>
+    <hyperlink ref="A7" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-854"/>
+    <hyperlink ref="A4" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-542"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed failed test case in IAM
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
   <si>
     <t>GET</t>
   </si>
@@ -181,19 +181,10 @@
     <t>X-1P-User=(SYS_USER2)</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>status=200||userid=(SYS_USER2)||preferredProvider=STEAM</t>
   </si>
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>status=200||notification=true</t>
   </si>
   <si>
     <t>status=200||recipient=(SYS_USER2)||email=(OPQA-542_email)||subject=Update from Project Neon</t>
@@ -203,13 +194,15 @@
   "userid": "(SYS_USER2)",
    "notifications": true
 }</t>
+  </si>
+  <si>
+    <t>status=200||notifications=true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -596,24 +589,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="33.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="58.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="79.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="6" width="70.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="6" width="70.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="6" width="43.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="26" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="58" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="79" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="70.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="70.28515625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="43.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -680,9 +673,6 @@
         <v>11</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
@@ -710,9 +700,6 @@
         <v>11</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
@@ -737,12 +724,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="1"/>
       <c r="J4" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -769,13 +753,8 @@
       <c r="H5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I5"/>
       <c r="J5" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="60">
@@ -799,15 +778,10 @@
       </c>
       <c r="G6"/>
       <c r="H6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6"/>
+        <v>54</v>
+      </c>
       <c r="J6" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="K6"/>
-      <c r="L6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30">
@@ -831,13 +805,8 @@
       </c>
       <c r="G7"/>
       <c r="H7"/>
-      <c r="I7"/>
       <c r="J7" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="135">
@@ -865,13 +834,8 @@
       <c r="H8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I8"/>
       <c r="J8" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="K8"/>
-      <c r="L8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="135">
@@ -899,13 +863,8 @@
       <c r="H9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I9"/>
       <c r="J9" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="K9"/>
-      <c r="L9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="135">
@@ -937,11 +896,7 @@
         <v>22</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Failing test scripts
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -148,9 +148,6 @@
     <t>?subject=Update from Project Neon&amp;template=summary-email.mustache&amp;html=true</t>
   </si>
   <si>
-    <t>status=403||errorcode=403||Reason=Invalid or Empty parameter</t>
-  </si>
-  <si>
     <t>/auth/email/(SYS_USER2)a</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>status=200||notifications=true</t>
+  </si>
+  <si>
+    <t>status=403||errorcode=403||Reason=Invalid/Empty parameter</t>
   </si>
 </sst>
 </file>
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L10"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,22 +712,22 @@
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="5"/>
       <c r="I4" s="1"/>
       <c r="J4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="105">
@@ -768,7 +768,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>21</v>
@@ -778,7 +778,7 @@
       </c>
       <c r="G6"/>
       <c r="H6" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>11</v>
@@ -795,32 +795,32 @@
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7"/>
       <c r="H7"/>
       <c r="J7" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="135">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>34</v>
@@ -840,16 +840,16 @@
     </row>
     <row r="9" spans="1:12" ht="135">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>34</v>
@@ -864,21 +864,21 @@
         <v>37</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="135">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>34</v>
@@ -896,7 +896,7 @@
         <v>22</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Test scripts into 1PAUTH module
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
   <si>
     <t>GET</t>
   </si>
@@ -197,6 +197,93 @@
   </si>
   <si>
     <t>status=403||errorcode=403||Reason=Invalid/Empty parameter</t>
+  </si>
+  <si>
+    <t>status=200||result=true||loginid=(OPQA-542_email)</t>
+  </si>
+  <si>
+    <t>/account/user/(OPQA-542_email)</t>
+  </si>
+  <si>
+    <t>/account/user/(OPQA-542_email)m</t>
+  </si>
+  <si>
+    <t>status=200||result=false||loginid=(OPQA-542_email)m</t>
+  </si>
+  <si>
+    <t>{"loginid":"(OPQA-542_email)","password":"1Platform!"}</t>
+  </si>
+  <si>
+    <t>status=200||userid=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>{"loginid":"(OPQA-542_email)","password":"1Platform"}</t>
+  </si>
+  <si>
+    <t>status=404||reason=Wrong user crendentials||errorcode=404</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>?app=neon</t>
+  </si>
+  <si>
+    <t>Verify that to test the authorize API for Redirection to Rest password page</t>
+  </si>
+  <si>
+    <t>/account/getsid</t>
+  </si>
+  <si>
+    <t>status=200||steamid=394389||truid=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>Verify that to get steamid by passing truid</t>
+  </si>
+  <si>
+    <t>Verify that to get error status for getting steam id  by passing wrong  truid</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)1</t>
+  </si>
+  <si>
+    <t>Verify that user able to login with valid credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that to get error status by passing wrong credentials </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that given mail id was registered with neon and validate response </t>
+  </si>
+  <si>
+    <t>OPQA-2704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that given mail id was not registered with neon and validate response </t>
+  </si>
+  <si>
+    <t>OPQA-2705</t>
+  </si>
+  <si>
+    <t>OPQA-2706</t>
+  </si>
+  <si>
+    <t>OPQA-2707</t>
+  </si>
+  <si>
+    <t>OPQA-2708</t>
+  </si>
+  <si>
+    <t>OPQA-2709</t>
+  </si>
+  <si>
+    <t>OPQA-2710</t>
+  </si>
+  <si>
+    <t>/account/resetpassword</t>
+  </si>
+  <si>
+    <t>status=401||reason=STeAM id is not found||errorcode=401</t>
   </si>
 </sst>
 </file>
@@ -587,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -899,6 +986,193 @@
         <v>52</v>
       </c>
     </row>
+    <row r="11" spans="1:12" ht="45">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13"/>
+      <c r="H13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14"/>
+      <c r="H14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15"/>
+      <c r="J15" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="J16" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="J17" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-540"/>

</xml_diff>

<commit_message>
Fixed Failing tests in IAM
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="92">
   <si>
     <t>GET</t>
   </si>
@@ -226,12 +226,6 @@
     <t>token</t>
   </si>
   <si>
-    <t>?app=neon</t>
-  </si>
-  <si>
-    <t>Verify that to test the authorize API for Redirection to Rest password page</t>
-  </si>
-  <si>
     <t>/account/getsid</t>
   </si>
   <si>
@@ -271,19 +265,46 @@
     <t>OPQA-2707</t>
   </si>
   <si>
-    <t>OPQA-2708</t>
-  </si>
-  <si>
     <t>OPQA-2709</t>
   </si>
   <si>
     <t>OPQA-2710</t>
   </si>
   <si>
-    <t>/account/resetpassword</t>
-  </si>
-  <si>
     <t>status=401||reason=STeAM id is not found||errorcode=401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that to validate existing token is valid or not </t>
+  </si>
+  <si>
+    <t>/validate/(OPQA-2706_token)</t>
+  </si>
+  <si>
+    <t>status=200||uid=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>Verify that to delete existing token.</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>/session/user/(SYS_USER2)/(OPQA-2706_token)</t>
+  </si>
+  <si>
+    <t>Verify that to get error status for  validating non existing token.</t>
+  </si>
+  <si>
+    <t>status=401</t>
+  </si>
+  <si>
+    <t>OPQA-2760</t>
+  </si>
+  <si>
+    <t>OPQA-2761</t>
+  </si>
+  <si>
+    <t>OPQA-2762</t>
   </si>
 </sst>
 </file>
@@ -359,7 +380,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -379,6 +400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -674,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L17"/>
+    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
+      <selection activeCell="L19" sqref="L2:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -988,10 +1010,10 @@
     </row>
     <row r="11" spans="1:12" ht="45">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -1013,10 +1035,10 @@
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -1038,10 +1060,10 @@
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -1071,10 +1093,10 @@
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -1099,78 +1121,129 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="45">
+    <row r="15" spans="1:12" ht="30">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="30">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
       <c r="J16" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30">
       <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F17" t="s">
-        <v>71</v>
-      </c>
       <c r="G17"/>
       <c r="H17"/>
+      <c r="I17" t="s">
+        <v>76</v>
+      </c>
       <c r="J17" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>84</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19" t="s">
+        <v>76</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test scripts in to IAM
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="112">
   <si>
     <t>GET</t>
   </si>
@@ -305,6 +305,66 @@
   </si>
   <si>
     <t>OPQA-2762</t>
+  </si>
+  <si>
+    <t>/admin/access</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER2)" ,"userStatus":"Deactivate", "comments":"Deactivate User"}</t>
+  </si>
+  <si>
+    <t>OPQA-543</t>
+  </si>
+  <si>
+    <t>Verify that to evict not-logged-in user and test whether that user is able to login or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that evicted user  not able to login with valid credentials </t>
+  </si>
+  <si>
+    <t>Verify that user is able to activate evicted user by passing truid</t>
+  </si>
+  <si>
+    <t>OPQA-746</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER2)" ,"userStatus":"Activate", "comments":"Activate evicted User"}</t>
+  </si>
+  <si>
+    <t>status=423||reason=User is evicted||errorcode=423</t>
+  </si>
+  <si>
+    <t>OPQA-544</t>
+  </si>
+  <si>
+    <t>OPQA-2706_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that system is ability to evict an already logged in user. </t>
+  </si>
+  <si>
+    <t>OPQA-544_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that to validate token which was evicted user who already login to neon </t>
+  </si>
+  <si>
+    <t>OPQA-544_2</t>
+  </si>
+  <si>
+    <t>OPQA-547</t>
+  </si>
+  <si>
+    <t>Verify whether reverted user able to log in or not. And test reverted user should able to login in to Neon</t>
+  </si>
+  <si>
+    <t>/validate/(OPQA-2706_1_token)</t>
+  </si>
+  <si>
+    <t>OPQA-745</t>
+  </si>
+  <si>
+    <t>status=423</t>
   </si>
 </sst>
 </file>
@@ -696,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="L19" sqref="L2:L19"/>
+    <sheetView tabSelected="1" topLeftCell="H21" workbookViewId="0">
+      <selection activeCell="L27" sqref="L2:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1171,7 +1231,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30">
+    <row r="17" spans="1:11" ht="30">
       <c r="A17" t="s">
         <v>89</v>
       </c>
@@ -1196,7 +1256,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="30">
+    <row r="18" spans="1:11" ht="30">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -1221,7 +1281,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30">
+    <row r="19" spans="1:11" ht="30">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -1244,6 +1304,232 @@
       </c>
       <c r="J19" s="6" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="45">
+      <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30">
+      <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21"/>
+      <c r="H21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23"/>
+      <c r="H23" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24"/>
+      <c r="H24" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="45">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26"/>
+      <c r="H26" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="60">
+      <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27"/>
+      <c r="H27" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests in to IAM
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="131">
   <si>
     <t>GET</t>
   </si>
@@ -365,6 +365,66 @@
   </si>
   <si>
     <t>status=423</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that to refresh token and validate new token generated or not </t>
+  </si>
+  <si>
+    <t>{
+  "uid": "(SYS_USER2)",
+  "token": "(OPQA-547_token)"
+}</t>
+  </si>
+  <si>
+    <t>OPQA-2777</t>
+  </si>
+  <si>
+    <t>/session/user/(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>/account/register/neon</t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)@sharklasers.com</t>
+  </si>
+  <si>
+    <t>truid</t>
+  </si>
+  <si>
+    <t>Verify that to register neon account using API</t>
+  </si>
+  <si>
+    <t>OPQA-2779</t>
+  </si>
+  <si>
+    <t>OPQA-2780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that neon API able to send verification email </t>
+  </si>
+  <si>
+    <t>/account/email/(OPQA-2779_truid)/activate</t>
+  </si>
+  <si>
+    <t>{"loginid":"(ddMMMyyyy_HHmmss)@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>status=403||errorcode=403||truid=(OPQA-2779_truid)||reason=Activate Registered account to continue</t>
+  </si>
+  <si>
+    <t>Content-Type=application/json||host=dev-stable.1p.thomsonreuters.com</t>
+  </si>
+  <si>
+    <t>status=400</t>
+  </si>
+  <si>
+    <t>Verify that to get error status not activated account.</t>
+  </si>
+  <si>
+    <t>OPQA-2782</t>
   </si>
 </sst>
 </file>
@@ -756,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H21" workbookViewId="0">
-      <selection activeCell="L27" sqref="L2:L27"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1531,6 +1591,130 @@
       <c r="J27" s="6" t="s">
         <v>61</v>
       </c>
+      <c r="K27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="60">
+      <c r="A28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="I28" t="s">
+        <v>107</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30">
+      <c r="A29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29"/>
+      <c r="H29" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="45">
+      <c r="A30" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30"/>
+      <c r="H30" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I30" t="s">
+        <v>121</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30">
+      <c r="A31" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" t="s">
+        <v>127</v>
+      </c>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31" t="s">
+        <v>121</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added test cases in Iam and Oauth APIs
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="229">
   <si>
     <t>GET</t>
   </si>
@@ -217,9 +217,6 @@
     <t>status=200||userid=(SYS_USER2)</t>
   </si>
   <si>
-    <t>{"loginid":"(OPQA-542_email)","password":"1Platform"}</t>
-  </si>
-  <si>
     <t>status=404||reason=Wrong user crendentials||errorcode=404</t>
   </si>
   <si>
@@ -422,13 +419,319 @@
   </si>
   <si>
     <t>OPQA-2782</t>
+  </si>
+  <si>
+    <t>Verify that to change user’s password  by passing valid password using 1PAuth API.</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing current password using 1PAuth API.</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing one of the previous password using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing empty password using 1PAuth API</t>
+  </si>
+  <si>
+    <t>/auth/account/password</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon@123" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123" }</t>
+  </si>
+  <si>
+    <t>OPQA-3479</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that system able to register new user using OAUTH API </t>
+  </si>
+  <si>
+    <t>1POAUTH</t>
+  </si>
+  <si>
+    <t>/user</t>
+  </si>
+  <si>
+    <t>{
+    "userName" : "(ddMMMyyyy_HHmmss)@tr.com",
+    "password" : "Neon@123",
+    "firstName" : "test",
+    "lastName" : "user",
+    "truid": "(UUID)"
+}</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||Reason=New password should not match current password</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||Reason=New password should not match previous 4 passwords</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||Reason=Password provided cannot be Empty</t>
+  </si>
+  <si>
+    <t>OPQA-2706_2</t>
+  </si>
+  <si>
+    <t>{"loginid":"(ddMMMyyyy_HHmmss)@tr.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>userid</t>
+  </si>
+  <si>
+    <t>X-1P-User=(OPQA-2706_2_userid)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||Reason=Password should contain at least one alphabet character, either upper or lower case</t>
+  </si>
+  <si>
+    <t>{ "password":"1234567890@" }</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password(numeric and special character) using 1PAuth API</t>
+  </si>
+  <si>
+    <t>{"loginid":"(OPQA-542_email)","password":"1Platform"}</t>
+  </si>
+  <si>
+    <t>{ "password":"" }</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400</t>
+  </si>
+  <si>
+    <t>{ "password":"123" }</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password using 1PAuth API</t>
+  </si>
+  <si>
+    <t>{ "password":"123@" }</t>
+  </si>
+  <si>
+    <t>{ "password":"ABCDEFG@" }</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||Reason=Password should have at least 1 numeric character</t>
+  </si>
+  <si>
+    <t>{ "password":"ABC@" }</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||Reason=Password should be at least 8 characters long||Reason=Password should have at least 1 numeric character</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||Reason=Password should be at least 8 characters long||Reason=Password should contain at least one alphabet character, either upper or lower case</t>
+  </si>
+  <si>
+    <t>OPQA-3757</t>
+  </si>
+  <si>
+    <t>OPQA-3758</t>
+  </si>
+  <si>
+    <t>OPQA-3759</t>
+  </si>
+  <si>
+    <t>OPQA-3760</t>
+  </si>
+  <si>
+    <t>OPQA-3761</t>
+  </si>
+  <si>
+    <t>OPQA-3762</t>
+  </si>
+  <si>
+    <t>OPQA-3763</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password(combination of alphabets and special characters) using 1PAuth API</t>
+  </si>
+  <si>
+    <t>OPQA-3764</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password(combination of alphabets and special characters below 8 characters) using 1PAuth API</t>
+  </si>
+  <si>
+    <t>OPQA-3765</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password(combination of numbers and special characters below 8 characters) using 1PAuth API</t>
+  </si>
+  <si>
+    <t>OPQA-3546</t>
+  </si>
+  <si>
+    <t>Verify that to register neon account with special symbol(+) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)+@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)+@sharklasers.com</t>
+  </si>
+  <si>
+    <t>OPQA-3547</t>
+  </si>
+  <si>
+    <t>Verify that to register neon account with special symbol(-) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)-@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)-@sharklasers.com</t>
+  </si>
+  <si>
+    <t>OPQA-3548</t>
+  </si>
+  <si>
+    <t>Verify that to register neon account with special symbols(.) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss).@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss).@sharklasers.com</t>
+  </si>
+  <si>
+    <t>OPQA-3549</t>
+  </si>
+  <si>
+    <t>Verify that to register neon account with special symbols( _) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)_@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)_@sharklasers.com</t>
+  </si>
+  <si>
+    <t>OPQA-3550</t>
+  </si>
+  <si>
+    <t>Verify that to register endnote account using 1P AUTH API</t>
+  </si>
+  <si>
+    <t>/account/register/endnote</t>
+  </si>
+  <si>
+    <t>OPQA-3551</t>
+  </si>
+  <si>
+    <t>Verify that to register EndNote account with special symbol(+) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>OPQA-3552</t>
+  </si>
+  <si>
+    <t>Verify that to register EndNote account with special symbol(-) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>OPQA-3553</t>
+  </si>
+  <si>
+    <t>Verify that to register EndNote account with special symbols(.) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>OPQA-3554</t>
+  </si>
+  <si>
+    <t>Verify that to register EndNote account with special symbols( _) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1+@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1-@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1.@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1_@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)1@sharklasers.com</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)1+@sharklasers.com</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)1-@sharklasers.com</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)1.@sharklasers.com</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)1_@sharklasers.com</t>
+  </si>
+  <si>
+    <t>OPQA-3561</t>
+  </si>
+  <si>
+    <t>Verify that to test the account API for Redirection to password reset page.</t>
+  </si>
+  <si>
+    <t>/account/resetpassword</t>
+  </si>
+  <si>
+    <t>OPQA-3562</t>
+  </si>
+  <si>
+    <t>Verify that to test the account API for Redirection to Shibboleth Login page</t>
+  </si>
+  <si>
+    <t>/account/shlogin</t>
+  </si>
+  <si>
+    <t>OPQA-3563</t>
+  </si>
+  <si>
+    <t>Verify that to get error status when user trying get account settings by passing wrong truid</t>
+  </si>
+  <si>
+    <t>status=400</t>
+  </si>
+  <si>
+    <t>OPQA-3564</t>
+  </si>
+  <si>
+    <t>Verify that to settings api able to change primary account.</t>
+  </si>
+  <si>
+    <t>status=200||message=Successfully updated user settings||status=200</t>
+  </si>
+  <si>
+    <t>{"preferredEmailProvider":"steam","userid":"2a326b50-2f08-11e6-a908-cd1e75e72744"}</t>
+  </si>
+  <si>
+    <t>{"preferredEmailProvider":"facebook","userid":"2a326b50-2f08-11e6-a908-cd1e75e72744"}</t>
+  </si>
+  <si>
+    <t>OPQA-3564_1</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the user password by passing wrong userid using 1PAuth API</t>
+  </si>
+  <si>
+    <t>X-1P-User=(OPQA-2706_2_userid)1||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>OPQA-3768</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,6 +753,13 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -497,7 +807,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -518,6 +828,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -813,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H26" workbookViewId="0">
-      <selection activeCell="L31" sqref="L2:L31"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L57" sqref="L2:L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1127,10 +1443,10 @@
     </row>
     <row r="11" spans="1:12" ht="45">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -1152,10 +1468,10 @@
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -1177,10 +1493,10 @@
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -1205,15 +1521,15 @@
         <v>61</v>
       </c>
       <c r="K13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -1229,27 +1545,27 @@
       </c>
       <c r="G14"/>
       <c r="H14" s="6" t="s">
-        <v>62</v>
+        <v>151</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>0</v>
@@ -1260,46 +1576,46 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
       <c r="J16" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>0</v>
@@ -1307,32 +1623,32 @@
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>11</v>
@@ -1340,16 +1656,16 @@
     </row>
     <row r="19" spans="1:11" ht="30">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>0</v>
@@ -1357,24 +1673,24 @@
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="45">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>21</v>
@@ -1384,7 +1700,7 @@
       </c>
       <c r="G20"/>
       <c r="H20" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>11</v>
@@ -1392,10 +1708,10 @@
     </row>
     <row r="21" spans="1:11" ht="30">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
@@ -1417,21 +1733,21 @@
         <v>22</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>21</v>
@@ -1441,7 +1757,7 @@
       </c>
       <c r="G22"/>
       <c r="H22" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>11</v>
@@ -1449,10 +1765,10 @@
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
@@ -1477,21 +1793,21 @@
         <v>61</v>
       </c>
       <c r="K23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="30">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>21</v>
@@ -1501,7 +1817,7 @@
       </c>
       <c r="G24"/>
       <c r="H24" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>11</v>
@@ -1509,16 +1825,16 @@
     </row>
     <row r="25" spans="1:11" ht="45">
       <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>0</v>
@@ -1526,24 +1842,24 @@
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="30">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>21</v>
@@ -1553,7 +1869,7 @@
       </c>
       <c r="G26"/>
       <c r="H26" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>11</v>
@@ -1561,10 +1877,10 @@
     </row>
     <row r="27" spans="1:11" ht="60">
       <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
@@ -1589,21 +1905,21 @@
         <v>61</v>
       </c>
       <c r="K27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60">
       <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>34</v>
@@ -1613,30 +1929,30 @@
       </c>
       <c r="G28"/>
       <c r="H28" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="30">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>34</v>
@@ -1646,21 +1962,21 @@
       </c>
       <c r="G29"/>
       <c r="H29" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="K29" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45">
       <c r="A30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -1676,41 +1992,767 @@
       </c>
       <c r="G30"/>
       <c r="H30" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I30" t="s">
+        <v>120</v>
+      </c>
+      <c r="J30" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="I30" t="s">
-        <v>121</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="A31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="105">
+      <c r="A32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32"/>
+      <c r="H32" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="30">
+      <c r="A33" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="I33" t="s">
+        <v>136</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="45">
+      <c r="A34" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G34"/>
+      <c r="H34" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="I34" t="s">
+        <v>144</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="60">
+      <c r="A35" t="s">
+        <v>228</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="G35"/>
+      <c r="H35" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="I35" t="s">
+        <v>144</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="45">
+      <c r="A36" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36"/>
+      <c r="H36" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="I36" t="s">
+        <v>144</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="60">
+      <c r="A37" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G37"/>
+      <c r="H37" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="I37" t="s">
+        <v>144</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="60">
+      <c r="A38" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G38"/>
+      <c r="H38" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="I38" t="s">
+        <v>144</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="45">
+      <c r="A39" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G39"/>
+      <c r="H39" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="I39" t="s">
+        <v>144</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="45">
+      <c r="A40" t="s">
+        <v>167</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G40"/>
+      <c r="H40" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="I40" t="s">
+        <v>144</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="90">
+      <c r="A41" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41"/>
+      <c r="H41" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="I41" t="s">
+        <v>144</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="75">
+      <c r="A42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G42"/>
+      <c r="H42" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="I42" t="s">
+        <v>144</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="90">
+      <c r="A43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G43"/>
+      <c r="H43" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="I43" t="s">
+        <v>144</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="45">
+      <c r="A44" t="s">
+        <v>174</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" t="s">
+        <v>35</v>
+      </c>
+      <c r="G44"/>
+      <c r="H44" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="45">
+      <c r="A45" t="s">
+        <v>178</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" t="s">
+        <v>35</v>
+      </c>
+      <c r="G45"/>
+      <c r="H45" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="45">
+      <c r="A46" t="s">
+        <v>182</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G46"/>
+      <c r="H46" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="45">
+      <c r="A47" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G47"/>
+      <c r="H47" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="30">
+      <c r="A48" t="s">
+        <v>190</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" t="s">
+        <v>35</v>
+      </c>
+      <c r="G48"/>
+      <c r="H48" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="45">
+      <c r="A49" t="s">
+        <v>193</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E49" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" t="s">
+        <v>35</v>
+      </c>
+      <c r="G49"/>
+      <c r="H49" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="45">
+      <c r="A50" t="s">
+        <v>195</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E50" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" t="s">
+        <v>35</v>
+      </c>
+      <c r="G50"/>
+      <c r="H50" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="45">
+      <c r="A51" t="s">
+        <v>197</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" t="s">
+        <v>35</v>
+      </c>
+      <c r="G51"/>
+      <c r="H51" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="45">
+      <c r="A52" t="s">
+        <v>199</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E52" t="s">
+        <v>34</v>
+      </c>
+      <c r="F52" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52"/>
+      <c r="H52" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="45">
+      <c r="A53" t="s">
+        <v>211</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="E53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="J53" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="45">
+      <c r="A54" t="s">
+        <v>214</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E54" t="s">
+        <v>0</v>
+      </c>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="J54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="45">
+      <c r="A55" t="s">
+        <v>217</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E55" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="J55" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="30">
+      <c r="A56" t="s">
+        <v>220</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F56" t="s">
+        <v>35</v>
+      </c>
+      <c r="G56"/>
+      <c r="H56" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="30">
+      <c r="A57" t="s">
+        <v>225</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E57" t="s">
+        <v>21</v>
+      </c>
+      <c r="F57" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57"/>
+      <c r="H57" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed shlogin test cases from Iam API
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="223">
   <si>
     <t>GET</t>
   </si>
@@ -673,24 +673,6 @@
     <t>status=200||email=(ddMMMyyyy_HHmmss)1_@sharklasers.com</t>
   </si>
   <si>
-    <t>OPQA-3561</t>
-  </si>
-  <si>
-    <t>Verify that to test the account API for Redirection to password reset page.</t>
-  </si>
-  <si>
-    <t>/account/resetpassword</t>
-  </si>
-  <si>
-    <t>OPQA-3562</t>
-  </si>
-  <si>
-    <t>Verify that to test the account API for Redirection to Shibboleth Login page</t>
-  </si>
-  <si>
-    <t>/account/shlogin</t>
-  </si>
-  <si>
     <t>OPQA-3563</t>
   </si>
   <si>
@@ -731,7 +713,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -753,13 +735,6 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -807,7 +782,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -830,9 +805,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1129,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L57" sqref="L2:L57"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2121,10 +2093,10 @@
     </row>
     <row r="35" spans="1:11" ht="60">
       <c r="A35" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C35" t="s">
         <v>14</v>
@@ -2136,7 +2108,7 @@
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
@@ -2636,52 +2608,60 @@
       <c r="A53" t="s">
         <v>211</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="6" t="s">
         <v>212</v>
       </c>
       <c r="C53" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>213</v>
+        <v>48</v>
       </c>
       <c r="E53" t="s">
         <v>0</v>
       </c>
+      <c r="F53" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="G53"/>
       <c r="H53"/>
-      <c r="J53" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="45">
+      <c r="J53" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="30">
       <c r="A54" t="s">
         <v>214</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="6" t="s">
         <v>215</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G54"/>
+      <c r="H54" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="J54" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E54" t="s">
-        <v>0</v>
-      </c>
-      <c r="G54"/>
-      <c r="H54"/>
-      <c r="J54" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="45">
+    </row>
+    <row r="55" spans="1:10" ht="30">
       <c r="A55" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
@@ -2690,69 +2670,17 @@
         <v>48</v>
       </c>
       <c r="E55" t="s">
-        <v>0</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>68</v>
+        <v>21</v>
+      </c>
+      <c r="F55" t="s">
+        <v>35</v>
       </c>
       <c r="G55"/>
-      <c r="H55"/>
-      <c r="J55" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="30">
-      <c r="A56" t="s">
-        <v>220</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C56" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E56" t="s">
-        <v>21</v>
-      </c>
-      <c r="F56" t="s">
-        <v>35</v>
-      </c>
-      <c r="G56"/>
-      <c r="H56" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="J56" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="30">
-      <c r="A57" t="s">
-        <v>225</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C57" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E57" t="s">
-        <v>21</v>
-      </c>
-      <c r="F57" t="s">
-        <v>35</v>
-      </c>
-      <c r="G57"/>
-      <c r="H57" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>222</v>
+      <c r="H55" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified stutus information in failed test case in IAMTestData excel
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -409,9 +409,6 @@
     <t>{"loginid":"(ddMMMyyyy_HHmmss)@sharklasers.com","password":"Neon@123"}</t>
   </si>
   <si>
-    <t>status=403||errorcode=403||truid=(OPQA-2779_truid)||reason=Activate Registered account to continue</t>
-  </si>
-  <si>
     <t>Content-Type=application/json||host=dev-stable.1p.thomsonreuters.com</t>
   </si>
   <si>
@@ -707,6 +704,9 @@
   </si>
   <si>
     <t>OPQA-3768</t>
+  </si>
+  <si>
+    <t>status=412||errorcode=412||truid=(OPQA-2779_truid)||reason=Activate Registered account to continue||status=accountNotActivated</t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="H20" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="G14"/>
       <c r="H14" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
@@ -1943,12 +1943,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="45">
+    <row r="30" spans="1:11" ht="60">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -1970,7 +1970,7 @@
         <v>120</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
@@ -1990,7 +1990,7 @@
         <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
@@ -2003,16 +2003,16 @@
     </row>
     <row r="32" spans="1:11" ht="105">
       <c r="A32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="C32" t="s">
         <v>137</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="9" t="s">
         <v>138</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>139</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>34</v>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>11</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>69</v>
@@ -2049,43 +2049,43 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="45">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G34"/>
       <c r="H34" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J34" s="6" t="s">
         <v>11</v>
@@ -2093,29 +2093,29 @@
     </row>
     <row r="35" spans="1:11" ht="60">
       <c r="A35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C35" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>38</v>
@@ -2123,250 +2123,250 @@
     </row>
     <row r="36" spans="1:11" ht="45">
       <c r="A36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60">
       <c r="A37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G37"/>
       <c r="H37" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60">
       <c r="A38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G38"/>
       <c r="H38" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="45">
       <c r="A39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="9" t="s">
         <v>132</v>
-      </c>
-      <c r="C39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>133</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="45">
       <c r="A40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="90">
       <c r="A41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="75">
       <c r="A42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="I42" t="s">
+        <v>143</v>
+      </c>
+      <c r="J42" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="I42" t="s">
-        <v>144</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="90">
       <c r="A43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="I43" t="s">
+        <v>143</v>
+      </c>
+      <c r="J43" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="I43" t="s">
-        <v>144</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="45">
       <c r="A44" t="s">
+        <v>173</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
@@ -2382,18 +2382,18 @@
       </c>
       <c r="G44"/>
       <c r="H44" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="J44" s="6" t="s">
         <v>176</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="45">
       <c r="A45" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
@@ -2409,18 +2409,18 @@
       </c>
       <c r="G45"/>
       <c r="H45" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="J45" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="45">
       <c r="A46" t="s">
+        <v>181</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>183</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
@@ -2436,18 +2436,18 @@
       </c>
       <c r="G46"/>
       <c r="H46" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="J46" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45">
       <c r="A47" t="s">
+        <v>185</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
@@ -2463,24 +2463,24 @@
       </c>
       <c r="G47"/>
       <c r="H47" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="30">
       <c r="A48" t="s">
+        <v>189</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="9" t="s">
         <v>191</v>
-      </c>
-      <c r="C48" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>192</v>
       </c>
       <c r="E48" t="s">
         <v>34</v>
@@ -2490,24 +2490,24 @@
       </c>
       <c r="G48"/>
       <c r="H48" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45">
       <c r="A49" t="s">
+        <v>192</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>194</v>
-      </c>
       <c r="C49" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E49" t="s">
         <v>34</v>
@@ -2517,24 +2517,24 @@
       </c>
       <c r="G49"/>
       <c r="H49" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45">
       <c r="A50" t="s">
+        <v>194</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="C50" t="s">
         <v>14</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E50" t="s">
         <v>34</v>
@@ -2544,24 +2544,24 @@
       </c>
       <c r="G50"/>
       <c r="H50" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="45">
       <c r="A51" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>198</v>
-      </c>
       <c r="C51" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E51" t="s">
         <v>34</v>
@@ -2571,24 +2571,24 @@
       </c>
       <c r="G51"/>
       <c r="H51" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45">
       <c r="A52" t="s">
+        <v>198</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>200</v>
-      </c>
       <c r="C52" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E52" t="s">
         <v>34</v>
@@ -2598,18 +2598,18 @@
       </c>
       <c r="G52"/>
       <c r="H52" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="45">
       <c r="A53" t="s">
+        <v>210</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="C53" t="s">
         <v>14</v>
@@ -2626,15 +2626,15 @@
       <c r="G53"/>
       <c r="H53"/>
       <c r="J53" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="30">
       <c r="A54" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
@@ -2650,18 +2650,18 @@
       </c>
       <c r="G54"/>
       <c r="H54" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30">
       <c r="A55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
@@ -2677,10 +2677,10 @@
       </c>
       <c r="G55"/>
       <c r="H55" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified test case validation in IAMTestData excel
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -706,7 +706,7 @@
     <t>OPQA-3768</t>
   </si>
   <si>
-    <t>status=412||errorcode=412||truid=(OPQA-2779_truid)||reason=Activate Registered account to continue||status=accountNotActivated</t>
+    <t>status=412||reason=Activate Registered account to continue||truid=(OPQA-2779_truid)||errorcode=412</t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H20" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1943,7 +1943,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="60">
+    <row r="30" spans="1:11" ht="45">
       <c r="A30" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
Modified Change password API test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="236">
   <si>
     <t>GET</t>
   </si>
@@ -418,27 +418,6 @@
     <t>OPQA-2782</t>
   </si>
   <si>
-    <t>Verify that to change user’s password  by passing valid password using 1PAuth API.</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing current password using 1PAuth API.</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing one of the previous password using 1PAuth API</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing empty password using 1PAuth API</t>
-  </si>
-  <si>
-    <t>/auth/account/password</t>
-  </si>
-  <si>
-    <t>{ "password":"Neon@123" }</t>
-  </si>
-  <si>
-    <t>{ "password":"Neon_123" }</t>
-  </si>
-  <si>
     <t>OPQA-3479</t>
   </si>
   <si>
@@ -460,15 +439,6 @@
 }</t>
   </si>
   <si>
-    <t>status=400||errorcode=400||Reason=New password should not match current password</t>
-  </si>
-  <si>
-    <t>status=400||errorcode=400||Reason=New password should not match previous 4 passwords</t>
-  </si>
-  <si>
-    <t>status=400||errorcode=400||Reason=Password provided cannot be Empty</t>
-  </si>
-  <si>
     <t>OPQA-2706_2</t>
   </si>
   <si>
@@ -481,48 +451,9 @@
     <t>X-1P-User=(OPQA-2706_2_userid)||Content-Type=application/json</t>
   </si>
   <si>
-    <t>status=400||errorcode=400||Reason=Password should contain at least one alphabet character, either upper or lower case</t>
-  </si>
-  <si>
-    <t>{ "password":"1234567890@" }</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing invalid password(numeric and special character) using 1PAuth API</t>
-  </si>
-  <si>
     <t>{"loginid":"(OPQA-542_email)","password":"1Platform"}</t>
   </si>
   <si>
-    <t>{ "password":"" }</t>
-  </si>
-  <si>
-    <t>status=400||errorcode=400</t>
-  </si>
-  <si>
-    <t>{ "password":"123" }</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing invalid password using 1PAuth API</t>
-  </si>
-  <si>
-    <t>{ "password":"123@" }</t>
-  </si>
-  <si>
-    <t>{ "password":"ABCDEFG@" }</t>
-  </si>
-  <si>
-    <t>status=400||errorcode=400||Reason=Password should have at least 1 numeric character</t>
-  </si>
-  <si>
-    <t>{ "password":"ABC@" }</t>
-  </si>
-  <si>
-    <t>status=400||errorcode=400||Reason=Password should be at least 8 characters long||Reason=Password should have at least 1 numeric character</t>
-  </si>
-  <si>
-    <t>status=400||errorcode=400||Reason=Password should be at least 8 characters long||Reason=Password should contain at least one alphabet character, either upper or lower case</t>
-  </si>
-  <si>
     <t>OPQA-3757</t>
   </si>
   <si>
@@ -544,21 +475,12 @@
     <t>OPQA-3763</t>
   </si>
   <si>
-    <t>Verify that to get error status while changing the password by passing invalid password(combination of alphabets and special characters) using 1PAuth API</t>
-  </si>
-  <si>
     <t>OPQA-3764</t>
   </si>
   <si>
-    <t>Verify that to get error status while changing the password by passing invalid password(combination of alphabets and special characters below 8 characters) using 1PAuth API</t>
-  </si>
-  <si>
     <t>OPQA-3765</t>
   </si>
   <si>
-    <t>Verify that to get error status while changing the password by passing invalid password(combination of numbers and special characters below 8 characters) using 1PAuth API</t>
-  </si>
-  <si>
     <t>OPQA-3546</t>
   </si>
   <si>
@@ -707,6 +629,123 @@
   </si>
   <si>
     <t>status=412||reason=Activate Registered account to continue||truid=(OPQA-2779_truid)||errorcode=412</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=422</t>
+  </si>
+  <si>
+    <t>status=200||message=Your password has been changed successfully!</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=422||reason=New password should not match current password</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=422||reason=New password should not match previous 4 passwords</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=422||reason=Password should be at least 8 characters long||reason=Password should contain at least one alphabet character, either upper or lower case</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||reason=Update request body is missing required parameters</t>
+  </si>
+  <si>
+    <t>status=422||reason=Password should contain at least one alphabet character, either upper or lower case</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=422||reason=Password should have at least 1 numeric character</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=422||reason=Password should be at least 8 characters long||reason=Password should have at least 1 numeric character</t>
+  </si>
+  <si>
+    <t>/account/auth/resetpassword</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon@123", "newpassword":"Neon_123" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"Neon_123" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"Neon@123" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"1234567890@" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"123" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"123@" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"ABCDEFG@" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"ABC@" }</t>
+  </si>
+  <si>
+    <t>status=404||errorcode=404||reason=Missing/Wrong user crendentials</t>
+  </si>
+  <si>
+    <t>status=401||errorcode=401||reason=STeAM id is not found</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the user password by passing empty userid using 1PAuth API</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||reason=Invalid or empty User ID</t>
+  </si>
+  <si>
+    <t>Verify that to change user’s password  by passing valid current password and new password using 1PAuth API.</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the user password by passing wrong current password using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing current password in new password paramenter using 1PAuth API.</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing one of the previous password in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password(numeric and special character) in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing empty password in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password(combination of numbers and special characters below 8 characters) in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password(combination of alphabets and special characters) in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password(combination of alphabets and special characters below 8 characters) in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing empty password in password parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>{ "password":" ", "newpassword":"Neon_123" }</t>
+  </si>
+  <si>
+    <t>X-1P-User=||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>OPQA-3907</t>
+  </si>
+  <si>
+    <t>OPQA-3908</t>
+  </si>
+  <si>
+    <t>OPQA-3909</t>
   </si>
 </sst>
 </file>
@@ -1101,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L67"/>
+    <sheetView tabSelected="1" topLeftCell="H53" workbookViewId="0">
+      <selection activeCell="L58" sqref="L2:L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1517,7 +1556,7 @@
       </c>
       <c r="G14"/>
       <c r="H14" s="6" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
@@ -1970,7 +2009,7 @@
         <v>120</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>222</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
@@ -2003,16 +2042,16 @@
     </row>
     <row r="32" spans="1:11" ht="105">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C32" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>34</v>
@@ -2022,7 +2061,7 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="6" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>11</v>
@@ -2030,7 +2069,7 @@
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>69</v>
@@ -2049,405 +2088,411 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="6" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="I33" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K33" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="60">
       <c r="A34" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>128</v>
+        <v>220</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G34"/>
       <c r="H34" s="6" t="s">
-        <v>134</v>
+        <v>207</v>
       </c>
       <c r="I34" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>11</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60">
       <c r="A35" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="C35" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
-        <v>134</v>
+        <v>207</v>
       </c>
       <c r="I35" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="45">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="60">
       <c r="A36" t="s">
-        <v>162</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>129</v>
+        <v>233</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>218</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>146</v>
+        <v>232</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="I36" t="s">
-        <v>143</v>
+        <v>207</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>140</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60">
       <c r="A37" t="s">
-        <v>163</v>
+        <v>234</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>130</v>
+        <v>221</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G37"/>
       <c r="H37" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I37" t="s">
         <v>133</v>
       </c>
-      <c r="I37" t="s">
-        <v>143</v>
-      </c>
       <c r="J37" s="6" t="s">
-        <v>141</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60">
       <c r="A38" t="s">
-        <v>164</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>149</v>
+        <v>139</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>222</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G38"/>
       <c r="H38" s="6" t="s">
-        <v>148</v>
+        <v>208</v>
       </c>
       <c r="I38" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="45">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="75">
       <c r="A39" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>131</v>
+        <v>223</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="6" t="s">
-        <v>151</v>
+        <v>209</v>
       </c>
       <c r="I39" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="75">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>154</v>
+        <v>224</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="6" t="s">
-        <v>153</v>
+        <v>210</v>
       </c>
       <c r="I40" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="90">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="60">
       <c r="A41" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>172</v>
+        <v>225</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="6" t="s">
-        <v>155</v>
+        <v>211</v>
       </c>
       <c r="I41" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="75">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="60">
       <c r="A42" t="s">
-        <v>169</v>
+        <v>235</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>168</v>
+        <v>230</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
-        <v>156</v>
+        <v>231</v>
       </c>
       <c r="I42" t="s">
+        <v>133</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="60">
+      <c r="A43" t="s">
         <v>143</v>
       </c>
-      <c r="J42" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="90">
-      <c r="A43" t="s">
-        <v>171</v>
-      </c>
       <c r="B43" s="6" t="s">
-        <v>170</v>
+        <v>226</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="6" t="s">
-        <v>158</v>
+        <v>212</v>
       </c>
       <c r="I43" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="45">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="105">
       <c r="A44" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>174</v>
+        <v>227</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E44" t="s">
-        <v>34</v>
-      </c>
-      <c r="F44" t="s">
-        <v>35</v>
+        <v>206</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="G44"/>
       <c r="H44" s="6" t="s">
-        <v>175</v>
+        <v>213</v>
+      </c>
+      <c r="I44" t="s">
+        <v>133</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="45">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="90">
       <c r="A45" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>178</v>
+        <v>228</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E45" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45" t="s">
-        <v>35</v>
+        <v>206</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="G45"/>
       <c r="H45" s="6" t="s">
-        <v>179</v>
+        <v>214</v>
+      </c>
+      <c r="I45" t="s">
+        <v>133</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="45">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="105">
       <c r="A46" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E46" t="s">
-        <v>34</v>
-      </c>
-      <c r="F46" t="s">
-        <v>35</v>
+        <v>206</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="G46"/>
       <c r="H46" s="6" t="s">
-        <v>183</v>
+        <v>215</v>
+      </c>
+      <c r="I46" t="s">
+        <v>133</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45">
       <c r="A47" t="s">
-        <v>185</v>
+        <v>147</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
@@ -2463,24 +2508,24 @@
       </c>
       <c r="G47"/>
       <c r="H47" s="6" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="30">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="45">
       <c r="A48" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>191</v>
+        <v>115</v>
       </c>
       <c r="E48" t="s">
         <v>34</v>
@@ -2490,24 +2535,24 @@
       </c>
       <c r="G48"/>
       <c r="H48" s="6" t="s">
-        <v>200</v>
+        <v>153</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>205</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45">
       <c r="A49" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="C49" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>191</v>
+        <v>115</v>
       </c>
       <c r="E49" t="s">
         <v>34</v>
@@ -2517,24 +2562,24 @@
       </c>
       <c r="G49"/>
       <c r="H49" s="6" t="s">
-        <v>201</v>
+        <v>157</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45">
       <c r="A50" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="C50" t="s">
         <v>14</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>191</v>
+        <v>115</v>
       </c>
       <c r="E50" t="s">
         <v>34</v>
@@ -2544,24 +2589,24 @@
       </c>
       <c r="G50"/>
       <c r="H50" s="6" t="s">
-        <v>202</v>
+        <v>161</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="45">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="30">
       <c r="A51" t="s">
-        <v>196</v>
+        <v>163</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
       <c r="C51" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="E51" t="s">
         <v>34</v>
@@ -2571,24 +2616,24 @@
       </c>
       <c r="G51"/>
       <c r="H51" s="6" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>208</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45">
       <c r="A52" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="C52" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="E52" t="s">
         <v>34</v>
@@ -2598,89 +2643,170 @@
       </c>
       <c r="G52"/>
       <c r="H52" s="6" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="45">
       <c r="A53" t="s">
-        <v>210</v>
+        <v>168</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>211</v>
+        <v>169</v>
       </c>
       <c r="C53" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="E53" t="s">
-        <v>0</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>68</v>
+        <v>34</v>
+      </c>
+      <c r="F53" t="s">
+        <v>35</v>
       </c>
       <c r="G53"/>
-      <c r="H53"/>
-      <c r="J53" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="30">
+      <c r="H53" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="45">
       <c r="A54" t="s">
-        <v>213</v>
+        <v>170</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>214</v>
+        <v>171</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="E54" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="F54" t="s">
         <v>35</v>
       </c>
       <c r="G54"/>
       <c r="H54" s="6" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="30">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="45">
       <c r="A55" t="s">
-        <v>218</v>
+        <v>172</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="E55" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="F55" t="s">
         <v>35</v>
       </c>
       <c r="G55"/>
       <c r="H55" s="6" t="s">
-        <v>217</v>
+        <v>178</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>215</v>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="45">
+      <c r="A56" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E56" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="J56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="30">
+      <c r="A57" t="s">
+        <v>187</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C57" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E57" t="s">
+        <v>21</v>
+      </c>
+      <c r="F57" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57"/>
+      <c r="H57" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="30">
+      <c r="A58" t="s">
+        <v>192</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" t="s">
+        <v>35</v>
+      </c>
+      <c r="G58"/>
+      <c r="H58" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="J58" s="6" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified 1PAuth error validations and watchlist services in Notify API
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -688,9 +688,6 @@
     <t>{ "password":"Neon_123", "newpassword":"ABC@" }</t>
   </si>
   <si>
-    <t>status=404||errorcode=404||reason=Missing/Wrong user crendentials</t>
-  </si>
-  <si>
     <t>status=401||errorcode=401||reason=STeAM id is not found</t>
   </si>
   <si>
@@ -746,6 +743,9 @@
   </si>
   <si>
     <t>OPQA-3909</t>
+  </si>
+  <si>
+    <t>status=404||errorcode=404||reason=Incorrect password. Please try again.</t>
   </si>
 </sst>
 </file>
@@ -1142,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H53" workbookViewId="0">
-      <selection activeCell="L58" sqref="L2:L58"/>
+    <sheetView tabSelected="1" topLeftCell="H33" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2105,7 +2105,7 @@
         <v>138</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
@@ -2157,15 +2157,15 @@
         <v>133</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60">
       <c r="A36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
@@ -2177,22 +2177,22 @@
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
         <v>207</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60">
       <c r="A37" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
@@ -2214,7 +2214,7 @@
         <v>133</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>216</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60">
@@ -2222,7 +2222,7 @@
         <v>139</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
@@ -2252,7 +2252,7 @@
         <v>140</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
@@ -2282,7 +2282,7 @@
         <v>141</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
@@ -2312,7 +2312,7 @@
         <v>142</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
@@ -2339,10 +2339,10 @@
     </row>
     <row r="42" spans="1:11" ht="60">
       <c r="A42" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
@@ -2358,7 +2358,7 @@
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I42" t="s">
         <v>133</v>
@@ -2372,7 +2372,7 @@
         <v>143</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
@@ -2402,7 +2402,7 @@
         <v>144</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
@@ -2432,7 +2432,7 @@
         <v>145</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
@@ -2462,7 +2462,7 @@
         <v>146</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Modified responce in testdata.xlsx for Oauth and 1pauth modules
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -217,9 +217,6 @@
     <t>status=200||userid=(SYS_USER2)</t>
   </si>
   <si>
-    <t>status=404||reason=Wrong user crendentials||errorcode=404</t>
-  </si>
-  <si>
     <t>token</t>
   </si>
   <si>
@@ -791,6 +788,9 @@
   </si>
   <si>
     <t>/account/resetpassword</t>
+  </si>
+  <si>
+    <t>status=404||reason=Steam login failed||errorcode=404</t>
   </si>
 </sst>
 </file>
@@ -1194,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H57" workbookViewId="0">
-      <selection activeCell="L61" sqref="L2:L61"/>
+    <sheetView tabSelected="1" topLeftCell="G12" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1506,10 +1506,10 @@
     </row>
     <row r="11" spans="1:12" ht="45">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -1531,10 +1531,10 @@
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -1556,10 +1556,10 @@
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -1584,15 +1584,15 @@
         <v>61</v>
       </c>
       <c r="K13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -1608,27 +1608,27 @@
       </c>
       <c r="G14"/>
       <c r="H14" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>62</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>0</v>
@@ -1639,46 +1639,46 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
       <c r="J16" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>0</v>
@@ -1686,32 +1686,32 @@
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>11</v>
@@ -1719,16 +1719,16 @@
     </row>
     <row r="19" spans="1:11" ht="30">
       <c r="A19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>0</v>
@@ -1736,24 +1736,24 @@
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="45">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>21</v>
@@ -1763,7 +1763,7 @@
       </c>
       <c r="G20"/>
       <c r="H20" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>11</v>
@@ -1771,10 +1771,10 @@
     </row>
     <row r="21" spans="1:11" ht="30">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
@@ -1796,21 +1796,21 @@
         <v>22</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>21</v>
@@ -1820,7 +1820,7 @@
       </c>
       <c r="G22"/>
       <c r="H22" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>11</v>
@@ -1828,10 +1828,10 @@
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
@@ -1856,21 +1856,21 @@
         <v>61</v>
       </c>
       <c r="K23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="30">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>21</v>
@@ -1880,7 +1880,7 @@
       </c>
       <c r="G24"/>
       <c r="H24" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>11</v>
@@ -1888,16 +1888,16 @@
     </row>
     <row r="25" spans="1:11" ht="45">
       <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>0</v>
@@ -1905,24 +1905,24 @@
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="30">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>21</v>
@@ -1932,7 +1932,7 @@
       </c>
       <c r="G26"/>
       <c r="H26" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>11</v>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="27" spans="1:11" ht="60">
       <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
@@ -1968,21 +1968,21 @@
         <v>61</v>
       </c>
       <c r="K27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60">
       <c r="A28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>114</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>34</v>
@@ -1992,30 +1992,30 @@
       </c>
       <c r="G28"/>
       <c r="H28" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="30">
       <c r="A29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>34</v>
@@ -2025,21 +2025,21 @@
       </c>
       <c r="G29"/>
       <c r="H29" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="K29" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -2055,38 +2055,38 @@
       </c>
       <c r="G30"/>
       <c r="H30" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="A31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>123</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>11</v>
@@ -2094,16 +2094,16 @@
     </row>
     <row r="32" spans="1:11" ht="105">
       <c r="A32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="C32" t="s">
         <v>129</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>131</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>34</v>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>11</v>
@@ -2121,10 +2121,10 @@
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
         <v>14</v>
@@ -2140,417 +2140,417 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="60">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G34"/>
       <c r="H34" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60">
       <c r="A35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C35" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60">
       <c r="A36" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60">
       <c r="A37" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G37"/>
       <c r="H37" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60">
       <c r="A38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G38"/>
       <c r="H38" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="75">
       <c r="A39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="75">
       <c r="A40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="60">
       <c r="A41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="60">
       <c r="A42" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="60">
       <c r="A43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="105">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G44"/>
       <c r="H44" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="90">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G45"/>
       <c r="H45" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="105">
       <c r="A46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G46"/>
       <c r="H46" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45">
       <c r="A47" t="s">
+        <v>146</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>148</v>
-      </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E47" t="s">
         <v>34</v>
@@ -2560,24 +2560,24 @@
       </c>
       <c r="G47"/>
       <c r="H47" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="45">
       <c r="A48" t="s">
+        <v>150</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>152</v>
-      </c>
       <c r="C48" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E48" t="s">
         <v>34</v>
@@ -2587,24 +2587,24 @@
       </c>
       <c r="G48"/>
       <c r="H48" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="J48" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45">
       <c r="A49" t="s">
+        <v>154</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>156</v>
-      </c>
       <c r="C49" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E49" t="s">
         <v>34</v>
@@ -2614,24 +2614,24 @@
       </c>
       <c r="G49"/>
       <c r="H49" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="J49" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45">
       <c r="A50" t="s">
+        <v>158</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>160</v>
-      </c>
       <c r="C50" t="s">
         <v>14</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E50" t="s">
         <v>34</v>
@@ -2641,24 +2641,24 @@
       </c>
       <c r="G50"/>
       <c r="H50" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="J50" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="30">
       <c r="A51" t="s">
+        <v>162</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="C51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="E51" t="s">
         <v>34</v>
@@ -2668,24 +2668,24 @@
       </c>
       <c r="G51"/>
       <c r="H51" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45">
       <c r="A52" t="s">
+        <v>165</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>167</v>
-      </c>
       <c r="C52" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E52" t="s">
         <v>34</v>
@@ -2695,24 +2695,24 @@
       </c>
       <c r="G52"/>
       <c r="H52" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="45">
       <c r="A53" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>169</v>
-      </c>
       <c r="C53" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E53" t="s">
         <v>34</v>
@@ -2722,24 +2722,24 @@
       </c>
       <c r="G53"/>
       <c r="H53" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="45">
       <c r="A54" t="s">
+        <v>169</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="B54" s="6" t="s">
-        <v>171</v>
-      </c>
       <c r="C54" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E54" t="s">
         <v>34</v>
@@ -2749,24 +2749,24 @@
       </c>
       <c r="G54"/>
       <c r="H54" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="45">
       <c r="A55" t="s">
+        <v>171</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>173</v>
-      </c>
       <c r="C55" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E55" t="s">
         <v>34</v>
@@ -2776,18 +2776,18 @@
       </c>
       <c r="G55"/>
       <c r="H55" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="45">
       <c r="A56" t="s">
+        <v>183</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
@@ -2799,20 +2799,20 @@
         <v>0</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G56"/>
       <c r="H56"/>
       <c r="J56" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="30">
       <c r="A57" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="C57" t="s">
         <v>14</v>
@@ -2828,18 +2828,18 @@
       </c>
       <c r="G57"/>
       <c r="H57" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30">
       <c r="A58" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C58" t="s">
         <v>14</v>
@@ -2855,24 +2855,24 @@
       </c>
       <c r="G58"/>
       <c r="H58" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="60">
       <c r="A59" t="s">
+        <v>244</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>246</v>
-      </c>
       <c r="C59" t="s">
         <v>14</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E59" t="s">
         <v>34</v>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="G59"/>
       <c r="H59" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J59" s="6" t="s">
         <v>11</v>
@@ -2890,16 +2890,16 @@
     </row>
     <row r="60" spans="1:10" ht="105">
       <c r="A60" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E60" t="s">
         <v>34</v>
@@ -2909,24 +2909,24 @@
       </c>
       <c r="G60"/>
       <c r="H60" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="J60" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="120">
       <c r="A61" t="s">
+        <v>239</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>241</v>
-      </c>
       <c r="C61" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E61" t="s">
         <v>34</v>
@@ -2936,10 +2936,10 @@
       </c>
       <c r="G61"/>
       <c r="H61" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="J61" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="J61" s="6" t="s">
-        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified response for testcase in IAMtestdata.xlsx file
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -223,9 +223,6 @@
     <t>/account/getsid</t>
   </si>
   <si>
-    <t>status=200||steamid=394389||truid=(SYS_USER2)</t>
-  </si>
-  <si>
     <t>Verify that to get steamid by passing truid</t>
   </si>
   <si>
@@ -791,6 +788,9 @@
   </si>
   <si>
     <t>status=404||reason=Steam login failed||errorcode=404</t>
+  </si>
+  <si>
+    <t>status=200||steamid=394389||truid=(SYS_USER2)||loginid=project.neon2@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1194,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G12" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="G11" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1506,10 +1506,10 @@
     </row>
     <row r="11" spans="1:12" ht="45">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -1531,10 +1531,10 @@
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -1556,10 +1556,10 @@
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -1589,10 +1589,10 @@
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -1608,21 +1608,21 @@
       </c>
       <c r="G14"/>
       <c r="H14" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
@@ -1639,15 +1639,15 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>64</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
@@ -1659,26 +1659,26 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
       <c r="J16" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>0</v>
@@ -1686,32 +1686,32 @@
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>11</v>
@@ -1719,16 +1719,16 @@
     </row>
     <row r="19" spans="1:11" ht="30">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>0</v>
@@ -1736,24 +1736,24 @@
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="45">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>21</v>
@@ -1763,7 +1763,7 @@
       </c>
       <c r="G20"/>
       <c r="H20" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>11</v>
@@ -1771,10 +1771,10 @@
     </row>
     <row r="21" spans="1:11" ht="30">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
@@ -1796,21 +1796,21 @@
         <v>22</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>21</v>
@@ -1820,7 +1820,7 @@
       </c>
       <c r="G22"/>
       <c r="H22" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>11</v>
@@ -1828,10 +1828,10 @@
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
@@ -1861,16 +1861,16 @@
     </row>
     <row r="24" spans="1:11" ht="30">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>21</v>
@@ -1880,7 +1880,7 @@
       </c>
       <c r="G24"/>
       <c r="H24" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>11</v>
@@ -1888,16 +1888,16 @@
     </row>
     <row r="25" spans="1:11" ht="45">
       <c r="A25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>103</v>
-      </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>0</v>
@@ -1905,24 +1905,24 @@
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="30">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>21</v>
@@ -1932,7 +1932,7 @@
       </c>
       <c r="G26"/>
       <c r="H26" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>11</v>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="27" spans="1:11" ht="60">
       <c r="A27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>106</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
@@ -1973,16 +1973,16 @@
     </row>
     <row r="28" spans="1:11" ht="60">
       <c r="A28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>34</v>
@@ -1992,13 +1992,13 @@
       </c>
       <c r="G28"/>
       <c r="H28" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K28" t="s">
         <v>62</v>
@@ -2006,16 +2006,16 @@
     </row>
     <row r="29" spans="1:11" ht="30">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>34</v>
@@ -2025,21 +2025,21 @@
       </c>
       <c r="G29"/>
       <c r="H29" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="K29" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -2055,38 +2055,38 @@
       </c>
       <c r="G30"/>
       <c r="H30" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="A31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>11</v>
@@ -2094,16 +2094,16 @@
     </row>
     <row r="32" spans="1:11" ht="105">
       <c r="A32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="C32" t="s">
         <v>128</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>34</v>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>11</v>
@@ -2121,10 +2121,10 @@
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
         <v>14</v>
@@ -2140,417 +2140,417 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="60">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G34"/>
       <c r="H34" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C35" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60">
       <c r="A36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60">
       <c r="A37" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G37"/>
       <c r="H37" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G38"/>
       <c r="H38" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="75">
       <c r="A39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="75">
       <c r="A40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="60">
       <c r="A41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="60">
       <c r="A42" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="60">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="105">
       <c r="A44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G44"/>
       <c r="H44" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="90">
       <c r="A45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G45"/>
       <c r="H45" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="105">
       <c r="A46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G46"/>
       <c r="H46" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45">
       <c r="A47" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>147</v>
-      </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E47" t="s">
         <v>34</v>
@@ -2560,24 +2560,24 @@
       </c>
       <c r="G47"/>
       <c r="H47" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="45">
       <c r="A48" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>151</v>
-      </c>
       <c r="C48" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E48" t="s">
         <v>34</v>
@@ -2587,24 +2587,24 @@
       </c>
       <c r="G48"/>
       <c r="H48" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J48" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45">
       <c r="A49" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>155</v>
-      </c>
       <c r="C49" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E49" t="s">
         <v>34</v>
@@ -2614,24 +2614,24 @@
       </c>
       <c r="G49"/>
       <c r="H49" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="J49" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45">
       <c r="A50" t="s">
+        <v>157</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>159</v>
-      </c>
       <c r="C50" t="s">
         <v>14</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E50" t="s">
         <v>34</v>
@@ -2641,24 +2641,24 @@
       </c>
       <c r="G50"/>
       <c r="H50" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="J50" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="30">
       <c r="A51" t="s">
+        <v>161</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>163</v>
-      </c>
-      <c r="C51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="E51" t="s">
         <v>34</v>
@@ -2668,24 +2668,24 @@
       </c>
       <c r="G51"/>
       <c r="H51" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45">
       <c r="A52" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>166</v>
-      </c>
       <c r="C52" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E52" t="s">
         <v>34</v>
@@ -2695,24 +2695,24 @@
       </c>
       <c r="G52"/>
       <c r="H52" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="45">
       <c r="A53" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>168</v>
-      </c>
       <c r="C53" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E53" t="s">
         <v>34</v>
@@ -2722,24 +2722,24 @@
       </c>
       <c r="G53"/>
       <c r="H53" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="45">
       <c r="A54" t="s">
+        <v>168</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B54" s="6" t="s">
-        <v>170</v>
-      </c>
       <c r="C54" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E54" t="s">
         <v>34</v>
@@ -2749,24 +2749,24 @@
       </c>
       <c r="G54"/>
       <c r="H54" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="45">
       <c r="A55" t="s">
+        <v>170</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>172</v>
-      </c>
       <c r="C55" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E55" t="s">
         <v>34</v>
@@ -2776,18 +2776,18 @@
       </c>
       <c r="G55"/>
       <c r="H55" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="45">
       <c r="A56" t="s">
+        <v>182</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
@@ -2799,20 +2799,20 @@
         <v>0</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G56"/>
       <c r="H56"/>
       <c r="J56" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="30">
       <c r="A57" t="s">
+        <v>185</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="C57" t="s">
         <v>14</v>
@@ -2828,18 +2828,18 @@
       </c>
       <c r="G57"/>
       <c r="H57" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30">
       <c r="A58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C58" t="s">
         <v>14</v>
@@ -2855,24 +2855,24 @@
       </c>
       <c r="G58"/>
       <c r="H58" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="60">
       <c r="A59" t="s">
+        <v>243</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>245</v>
-      </c>
       <c r="C59" t="s">
         <v>14</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E59" t="s">
         <v>34</v>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="G59"/>
       <c r="H59" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J59" s="6" t="s">
         <v>11</v>
@@ -2890,16 +2890,16 @@
     </row>
     <row r="60" spans="1:10" ht="105">
       <c r="A60" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E60" t="s">
         <v>34</v>
@@ -2909,24 +2909,24 @@
       </c>
       <c r="G60"/>
       <c r="H60" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J60" s="6" t="s">
         <v>237</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="120">
       <c r="A61" t="s">
+        <v>238</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>240</v>
-      </c>
       <c r="C61" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E61" t="s">
         <v>34</v>
@@ -2936,10 +2936,10 @@
       </c>
       <c r="G61"/>
       <c r="H61" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="J61" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="J61" s="6" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the failed scripts in 1pAuth api
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="252">
   <si>
     <t>GET</t>
   </si>
@@ -148,12 +148,6 @@
     <t>?subject=Update from Project Neon&amp;template=summary-email.mustache&amp;html=true</t>
   </si>
   <si>
-    <t>/auth/email/(SYS_USER2)a</t>
-  </si>
-  <si>
-    <t>/auth/email/(SYS_USER2)</t>
-  </si>
-  <si>
     <t>Verify that to send update mails from neon</t>
   </si>
   <si>
@@ -791,6 +785,15 @@
   </si>
   <si>
     <t>status=200||steamid=394389||truid=(SYS_USER2)||loginid=project.neon2@gmail.com</t>
+  </si>
+  <si>
+    <t>x-1p-zuul-host=http://dev.1p.clarivate.com</t>
+  </si>
+  <si>
+    <t>/account/email/(SYS_USER2)a</t>
+  </si>
+  <si>
+    <t>/account/email/(SYS_USER2)</t>
   </si>
 </sst>
 </file>
@@ -1194,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G11" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1268,7 +1271,9 @@
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>249</v>
+      </c>
       <c r="G2" s="8" t="s">
         <v>16</v>
       </c>
@@ -1295,7 +1300,9 @@
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>249</v>
+      </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
       </c>
@@ -1317,22 +1324,22 @@
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="5"/>
       <c r="I4" s="1"/>
       <c r="J4" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="105">
@@ -1373,7 +1380,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>21</v>
@@ -1383,7 +1390,7 @@
       </c>
       <c r="G6"/>
       <c r="H6" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>11</v>
@@ -1400,32 +1407,32 @@
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G7"/>
       <c r="H7"/>
       <c r="J7" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="135">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>34</v>
@@ -1445,23 +1452,20 @@
     </row>
     <row r="9" spans="1:12" ht="135">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>251</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
       <c r="G9" s="6" t="s">
         <v>39</v>
       </c>
@@ -1469,21 +1473,21 @@
         <v>37</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="135">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>251</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>34</v>
@@ -1501,21 +1505,21 @@
         <v>22</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>0</v>
@@ -1526,21 +1530,21 @@
         <v>22</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>0</v>
@@ -1551,15 +1555,15 @@
         <v>22</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -1575,24 +1579,24 @@
       </c>
       <c r="G13"/>
       <c r="H13" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I13" t="s">
         <v>22</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -1608,77 +1612,77 @@
       </c>
       <c r="G14"/>
       <c r="H14" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
       <c r="J16" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>0</v>
@@ -1686,32 +1690,32 @@
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>83</v>
-      </c>
       <c r="E18" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>11</v>
@@ -1719,16 +1723,16 @@
     </row>
     <row r="19" spans="1:11" ht="30">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>0</v>
@@ -1736,24 +1740,24 @@
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="45">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>21</v>
@@ -1763,7 +1767,7 @@
       </c>
       <c r="G20"/>
       <c r="H20" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>11</v>
@@ -1771,10 +1775,10 @@
     </row>
     <row r="21" spans="1:11" ht="30">
       <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
@@ -1790,27 +1794,27 @@
       </c>
       <c r="G21"/>
       <c r="H21" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I21" t="s">
         <v>22</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>21</v>
@@ -1820,7 +1824,7 @@
       </c>
       <c r="G22"/>
       <c r="H22" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>11</v>
@@ -1828,10 +1832,10 @@
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
@@ -1847,30 +1851,30 @@
       </c>
       <c r="G23"/>
       <c r="H23" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I23" t="s">
         <v>22</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="30">
       <c r="A24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>100</v>
-      </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>21</v>
@@ -1880,7 +1884,7 @@
       </c>
       <c r="G24"/>
       <c r="H24" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>11</v>
@@ -1888,16 +1892,16 @@
     </row>
     <row r="25" spans="1:11" ht="45">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>0</v>
@@ -1905,24 +1909,24 @@
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="30">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>21</v>
@@ -1932,7 +1936,7 @@
       </c>
       <c r="G26"/>
       <c r="H26" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>11</v>
@@ -1940,10 +1944,10 @@
     </row>
     <row r="27" spans="1:11" ht="60">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
@@ -1959,30 +1963,30 @@
       </c>
       <c r="G27"/>
       <c r="H27" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I27" t="s">
         <v>22</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>34</v>
@@ -1992,30 +1996,30 @@
       </c>
       <c r="G28"/>
       <c r="H28" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="30">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>34</v>
@@ -2025,21 +2029,21 @@
       </c>
       <c r="G29"/>
       <c r="H29" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="K29" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -2055,38 +2059,38 @@
       </c>
       <c r="G30"/>
       <c r="H30" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="A31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>119</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>121</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>11</v>
@@ -2094,16 +2098,16 @@
     </row>
     <row r="32" spans="1:11" ht="105">
       <c r="A32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="D32" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="C32" t="s">
-        <v>128</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>34</v>
@@ -2113,7 +2117,7 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>11</v>
@@ -2121,10 +2125,10 @@
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
         <v>14</v>
@@ -2140,417 +2144,417 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="60">
       <c r="A34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G34"/>
       <c r="H34" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60">
       <c r="A35" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C35" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I35" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60">
       <c r="A36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60">
       <c r="A37" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G37"/>
       <c r="H37" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I37" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60">
       <c r="A38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G38"/>
       <c r="H38" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="75">
       <c r="A39" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="75">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I40" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="60">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I41" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="60">
       <c r="A42" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I42" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="60">
       <c r="A43" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I43" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="105">
       <c r="A44" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G44"/>
       <c r="H44" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I44" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="90">
       <c r="A45" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G45"/>
       <c r="H45" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I45" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="105">
       <c r="A46" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G46"/>
       <c r="H46" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I46" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E47" t="s">
         <v>34</v>
@@ -2560,24 +2564,24 @@
       </c>
       <c r="G47"/>
       <c r="H47" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="45">
       <c r="A48" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E48" t="s">
         <v>34</v>
@@ -2587,24 +2591,24 @@
       </c>
       <c r="G48"/>
       <c r="H48" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="45">
       <c r="A49" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C49" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E49" t="s">
         <v>34</v>
@@ -2614,24 +2618,24 @@
       </c>
       <c r="G49"/>
       <c r="H49" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="45">
       <c r="A50" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C50" t="s">
         <v>14</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E50" t="s">
         <v>34</v>
@@ -2641,24 +2645,24 @@
       </c>
       <c r="G50"/>
       <c r="H50" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="30">
       <c r="A51" t="s">
+        <v>159</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="C51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="E51" t="s">
         <v>34</v>
@@ -2668,24 +2672,24 @@
       </c>
       <c r="G51"/>
       <c r="H51" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="45">
       <c r="A52" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C52" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E52" t="s">
         <v>34</v>
@@ -2695,24 +2699,24 @@
       </c>
       <c r="G52"/>
       <c r="H52" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="45">
       <c r="A53" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C53" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E53" t="s">
         <v>34</v>
@@ -2722,24 +2726,24 @@
       </c>
       <c r="G53"/>
       <c r="H53" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="45">
       <c r="A54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E54" t="s">
         <v>34</v>
@@ -2749,24 +2753,24 @@
       </c>
       <c r="G54"/>
       <c r="H54" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="45">
       <c r="A55" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E55" t="s">
         <v>34</v>
@@ -2776,49 +2780,49 @@
       </c>
       <c r="G55"/>
       <c r="H55" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="45">
       <c r="A56" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E56" t="s">
         <v>0</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G56"/>
       <c r="H56"/>
       <c r="J56" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="30">
       <c r="A57" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C57" t="s">
         <v>14</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E57" t="s">
         <v>21</v>
@@ -2828,24 +2832,24 @@
       </c>
       <c r="G57"/>
       <c r="H57" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30">
       <c r="A58" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C58" t="s">
         <v>14</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E58" t="s">
         <v>21</v>
@@ -2855,24 +2859,24 @@
       </c>
       <c r="G58"/>
       <c r="H58" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="60">
       <c r="A59" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B59" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="9" t="s">
         <v>244</v>
-      </c>
-      <c r="C59" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>246</v>
       </c>
       <c r="E59" t="s">
         <v>34</v>
@@ -2882,7 +2886,7 @@
       </c>
       <c r="G59"/>
       <c r="H59" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J59" s="6" t="s">
         <v>11</v>
@@ -2890,16 +2894,16 @@
     </row>
     <row r="60" spans="1:10" ht="105">
       <c r="A60" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E60" t="s">
         <v>34</v>
@@ -2909,24 +2913,24 @@
       </c>
       <c r="G60"/>
       <c r="H60" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="120">
       <c r="A61" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E61" t="s">
         <v>34</v>
@@ -2936,10 +2940,10 @@
       </c>
       <c r="G61"/>
       <c r="H61" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified test data in IAM testdata file
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -781,9 +781,6 @@
     <t>/account/resetpassword</t>
   </si>
   <si>
-    <t>status=404||reason=Steam login failed||errorcode=404</t>
-  </si>
-  <si>
     <t>status=200||steamid=394389||truid=(SYS_USER2)||loginid=project.neon2@gmail.com</t>
   </si>
   <si>
@@ -794,6 +791,9 @@
   </si>
   <si>
     <t>/account/email/(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>status=404||reason=Missing/Wrong user crendentials||errorcode=404</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1198,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L67"/>
+      <selection activeCell="L2" sqref="L2:L106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1272,7 +1272,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>16</v>
@@ -1301,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
@@ -1432,7 +1432,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>34</v>
@@ -1461,7 +1461,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>34</v>
@@ -1487,7 +1487,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>34</v>
@@ -1618,7 +1618,7 @@
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
@@ -1643,7 +1643,7 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45">

</xml_diff>

<commit_message>
Added new testcases in IAM module
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="IAM" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="265">
   <si>
     <t>GET</t>
   </si>
@@ -795,12 +796,51 @@
   <si>
     <t>status=404||reason=Missing/Wrong user crendentials||errorcode=404</t>
   </si>
+  <si>
+    <t>OPQA-5579</t>
+  </si>
+  <si>
+    <t>Verify that valid short term token is able to generate using 1pAuth API</t>
+  </si>
+  <si>
+    <t>?provider=steam</t>
+  </si>
+  <si>
+    <t>{"loginid":"project.neon2@gmail.com","password":"1Platform!"}</t>
+  </si>
+  <si>
+    <t>status=200||provider=STEAM</t>
+  </si>
+  <si>
+    <t>OPQA-5580</t>
+  </si>
+  <si>
+    <t>Verify that valid long term token is generated by using short term token</t>
+  </si>
+  <si>
+    <t>/session/user/(OPQA-5579_token)</t>
+  </si>
+  <si>
+    <t>token||userid</t>
+  </si>
+  <si>
+    <t>status=200||userid=(OPQA-5579_userid)</t>
+  </si>
+  <si>
+    <t>OPQA-5581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that to get error status for  invalid long term token </t>
+  </si>
+  <si>
+    <t>/session/user/eyJ0eXAiOiJKiJ9eyJzdWIiOiIxNzRjMWF.tyyioikok</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,6 +866,25 @@
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -875,7 +934,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -900,6 +959,11 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1195,10 +1259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L106"/>
+    <sheetView tabSelected="1" topLeftCell="H61" workbookViewId="0">
+      <selection activeCell="L64" sqref="L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2597,7 +2661,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="45">
+    <row r="49" spans="1:11" ht="45">
       <c r="A49" t="s">
         <v>151</v>
       </c>
@@ -2624,7 +2688,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="45">
+    <row r="50" spans="1:11" ht="45">
       <c r="A50" t="s">
         <v>155</v>
       </c>
@@ -2651,7 +2715,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="30">
+    <row r="51" spans="1:11" ht="30">
       <c r="A51" t="s">
         <v>159</v>
       </c>
@@ -2678,7 +2742,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="45">
+    <row r="52" spans="1:11" ht="45">
       <c r="A52" t="s">
         <v>162</v>
       </c>
@@ -2705,7 +2769,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="45">
+    <row r="53" spans="1:11" ht="45">
       <c r="A53" t="s">
         <v>164</v>
       </c>
@@ -2732,7 +2796,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="45">
+    <row r="54" spans="1:11" ht="45">
       <c r="A54" t="s">
         <v>166</v>
       </c>
@@ -2759,7 +2823,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="45">
+    <row r="55" spans="1:11" ht="45">
       <c r="A55" t="s">
         <v>168</v>
       </c>
@@ -2786,7 +2850,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="45">
+    <row r="56" spans="1:11" ht="45">
       <c r="A56" t="s">
         <v>180</v>
       </c>
@@ -2811,7 +2875,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="30">
+    <row r="57" spans="1:11" ht="30">
       <c r="A57" t="s">
         <v>183</v>
       </c>
@@ -2838,7 +2902,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="30">
+    <row r="58" spans="1:11" ht="30">
       <c r="A58" t="s">
         <v>188</v>
       </c>
@@ -2865,7 +2929,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="60">
+    <row r="59" spans="1:11" ht="60">
       <c r="A59" t="s">
         <v>241</v>
       </c>
@@ -2892,7 +2956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="105">
+    <row r="60" spans="1:11" ht="105">
       <c r="A60" t="s">
         <v>233</v>
       </c>
@@ -2919,7 +2983,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="120">
+    <row r="61" spans="1:11" ht="120">
       <c r="A61" t="s">
         <v>236</v>
       </c>
@@ -2944,6 +3008,85 @@
       </c>
       <c r="J61" s="6" t="s">
         <v>240</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="30">
+      <c r="A62" t="s">
+        <v>252</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="C62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" t="s">
+        <v>34</v>
+      </c>
+      <c r="F62" t="s">
+        <v>35</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="J62" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="K62" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="45">
+      <c r="A63" t="s">
+        <v>257</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="E63" t="s">
+        <v>0</v>
+      </c>
+      <c r="G63"/>
+      <c r="H63"/>
+      <c r="J63" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="K63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="30">
+      <c r="A64" t="s">
+        <v>262</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E64" t="s">
+        <v>0</v>
+      </c>
+      <c r="G64"/>
+      <c r="H64"/>
+      <c r="J64" s="6" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2958,4 +3101,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed validations in IAMTestData.xlsx
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -620,33 +620,12 @@
     <t>status=412||reason=Activate Registered account to continue||truid=(OPQA-2779_truid)||errorcode=412</t>
   </si>
   <si>
-    <t>status=422||errorcode=422</t>
-  </si>
-  <si>
     <t>status=200||message=Your password has been changed successfully!</t>
   </si>
   <si>
-    <t>status=422||errorcode=422||reason=New password should not match current password</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=422||reason=New password should not match previous 4 passwords</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=422||reason=Password should be at least 8 characters long||reason=Password should contain at least one alphabet character, either upper or lower case</t>
-  </si>
-  <si>
-    <t>status=400||errorcode=400||reason=Update request body is missing required parameters</t>
-  </si>
-  <si>
     <t>status=422||reason=Password should contain at least one alphabet character, either upper or lower case</t>
   </si>
   <si>
-    <t>status=422||errorcode=422||reason=Password should have at least 1 numeric character</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=422||reason=Password should be at least 8 characters long||reason=Password should have at least 1 numeric character</t>
-  </si>
-  <si>
     <t>/account/auth/resetpassword</t>
   </si>
   <si>
@@ -834,6 +813,27 @@
   </si>
   <si>
     <t>/session/user/eyJ0eXAiOiJKiJ9eyJzdWIiOiIxNzRjMWF.tyyioikok</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=0||reason=New password should not match current password</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=0||reason=New password should not match previous 4 passwords</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=0||reason=Update request body is missing required parameters</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=0</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=0||reason=Password should be at least 8 characters long||reason=Password should contain at least one alphabet character, either upper or lower case</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=0||reason=Password should have at least 1 numeric character</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=0||reason=Password should be at least 8 characters long||reason=Password should have at least 1 numeric character</t>
   </si>
 </sst>
 </file>
@@ -1261,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H61" workbookViewId="0">
-      <selection activeCell="L64" sqref="L64"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1336,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>16</v>
@@ -1365,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
@@ -1496,7 +1496,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>34</v>
@@ -1525,7 +1525,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>34</v>
@@ -1551,7 +1551,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>34</v>
@@ -1682,7 +1682,7 @@
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
@@ -1707,7 +1707,7 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45">
@@ -1757,7 +1757,7 @@
         <v>71</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30">
@@ -2225,13 +2225,13 @@
         <v>134</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>21</v>
@@ -2241,13 +2241,13 @@
       </c>
       <c r="G34"/>
       <c r="H34" s="6" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="I34" t="s">
         <v>129</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60">
@@ -2261,7 +2261,7 @@
         <v>14</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>21</v>
@@ -2271,54 +2271,54 @@
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="I35" t="s">
         <v>129</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60">
       <c r="A36" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60">
       <c r="A37" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>21</v>
@@ -2328,13 +2328,13 @@
       </c>
       <c r="G37"/>
       <c r="H37" s="6" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="I37" t="s">
         <v>129</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60">
@@ -2342,13 +2342,13 @@
         <v>135</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>21</v>
@@ -2358,13 +2358,13 @@
       </c>
       <c r="G38"/>
       <c r="H38" s="6" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I38" t="s">
         <v>129</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>195</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="75">
@@ -2372,13 +2372,13 @@
         <v>136</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>21</v>
@@ -2388,13 +2388,13 @@
       </c>
       <c r="G39"/>
       <c r="H39" s="6" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I39" t="s">
         <v>129</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>196</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="75">
@@ -2402,13 +2402,13 @@
         <v>137</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>21</v>
@@ -2418,13 +2418,13 @@
       </c>
       <c r="G40"/>
       <c r="H40" s="6" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="I40" t="s">
         <v>129</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="60">
@@ -2432,13 +2432,13 @@
         <v>138</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>21</v>
@@ -2448,27 +2448,27 @@
       </c>
       <c r="G41"/>
       <c r="H41" s="6" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="I41" t="s">
         <v>129</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>198</v>
+        <v>260</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="60">
       <c r="A42" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>21</v>
@@ -2478,13 +2478,13 @@
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="I42" t="s">
         <v>129</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>198</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="60">
@@ -2492,13 +2492,13 @@
         <v>139</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
@@ -2508,13 +2508,13 @@
       </c>
       <c r="G43"/>
       <c r="H43" s="6" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="I43" t="s">
         <v>129</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>193</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="105">
@@ -2522,13 +2522,13 @@
         <v>140</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>21</v>
@@ -2538,13 +2538,13 @@
       </c>
       <c r="G44"/>
       <c r="H44" s="6" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="I44" t="s">
         <v>129</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>197</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="90">
@@ -2552,13 +2552,13 @@
         <v>141</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>21</v>
@@ -2568,13 +2568,13 @@
       </c>
       <c r="G45"/>
       <c r="H45" s="6" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="I45" t="s">
         <v>129</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>200</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="105">
@@ -2582,13 +2582,13 @@
         <v>142</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>21</v>
@@ -2598,13 +2598,13 @@
       </c>
       <c r="G46"/>
       <c r="H46" s="6" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="I46" t="s">
         <v>129</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>201</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45">
@@ -2931,16 +2931,16 @@
     </row>
     <row r="59" spans="1:11" ht="60">
       <c r="A59" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C59" t="s">
         <v>14</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E59" t="s">
         <v>34</v>
@@ -2950,7 +2950,7 @@
       </c>
       <c r="G59"/>
       <c r="H59" s="11" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="J59" s="6" t="s">
         <v>11</v>
@@ -2958,16 +2958,16 @@
     </row>
     <row r="60" spans="1:11" ht="105">
       <c r="A60" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B60" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="9" t="s">
         <v>238</v>
-      </c>
-      <c r="C60" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>245</v>
       </c>
       <c r="E60" t="s">
         <v>34</v>
@@ -2977,24 +2977,24 @@
       </c>
       <c r="G60"/>
       <c r="H60" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="120">
       <c r="A61" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E61" t="s">
         <v>34</v>
@@ -3004,18 +3004,18 @@
       </c>
       <c r="G61"/>
       <c r="H61" s="6" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="30">
       <c r="A62" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -3030,30 +3030,30 @@
         <v>35</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="K62" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="45">
       <c r="A63" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C63" t="s">
         <v>14</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E63" t="s">
         <v>0</v>
@@ -3061,7 +3061,7 @@
       <c r="G63"/>
       <c r="H63"/>
       <c r="J63" s="6" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="K63" t="s">
         <v>60</v>
@@ -3069,16 +3069,16 @@
     </row>
     <row r="64" spans="1:11" ht="30">
       <c r="A64" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C64" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E64" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed failed scripts in IAM module
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -611,9 +611,6 @@
     <t>Verify that to get error status while changing the user password by passing wrong userid using 1PAuth API</t>
   </si>
   <si>
-    <t>X-1P-User=(OPQA-2706_2_userid)1||Content-Type=application/json</t>
-  </si>
-  <si>
     <t>OPQA-3768</t>
   </si>
   <si>
@@ -788,9 +785,6 @@
     <t>{"loginid":"project.neon2@gmail.com","password":"1Platform!"}</t>
   </si>
   <si>
-    <t>status=200||provider=STEAM</t>
-  </si>
-  <si>
     <t>OPQA-5580</t>
   </si>
   <si>
@@ -834,6 +828,12 @@
   </si>
   <si>
     <t>status=422||errorcode=0||reason=Password should be at least 8 characters long||reason=Password should have at least 1 numeric character</t>
+  </si>
+  <si>
+    <t>X-1P-User=(OPQA-2706_2_userid)||Content-Type=application/json||x-1p-zuul-host=http://localhost:7001</t>
+  </si>
+  <si>
+    <t>X-1P-User=(OPQA-2706_2_userid)1||Content-Type=application/json||x-1p-zuul-host=http://localhost:7001</t>
   </si>
 </sst>
 </file>
@@ -1262,7 +1262,7 @@
   <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="L2" sqref="L2:L89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1336,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>16</v>
@@ -1365,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
@@ -1496,7 +1496,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>34</v>
@@ -1525,7 +1525,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>34</v>
@@ -1551,7 +1551,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>34</v>
@@ -1682,7 +1682,7 @@
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
@@ -1707,7 +1707,7 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45">
@@ -1757,7 +1757,7 @@
         <v>71</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30">
@@ -2129,7 +2129,7 @@
         <v>116</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
@@ -2225,34 +2225,34 @@
         <v>134</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="G34"/>
       <c r="H34" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I34" t="s">
         <v>129</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60">
       <c r="A35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>189</v>
@@ -2261,80 +2261,80 @@
         <v>14</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>190</v>
+        <v>264</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I35" t="s">
         <v>129</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60">
       <c r="A36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60">
       <c r="A37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="G37"/>
       <c r="H37" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I37" t="s">
         <v>129</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60">
@@ -2342,29 +2342,29 @@
         <v>135</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="G38"/>
       <c r="H38" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I38" t="s">
         <v>129</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="75">
@@ -2372,29 +2372,29 @@
         <v>136</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I39" t="s">
         <v>129</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="75">
@@ -2402,29 +2402,29 @@
         <v>137</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I40" t="s">
         <v>129</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="60">
@@ -2432,13 +2432,13 @@
         <v>138</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>21</v>
@@ -2448,27 +2448,27 @@
       </c>
       <c r="G41"/>
       <c r="H41" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I41" t="s">
         <v>129</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="60">
       <c r="A42" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>21</v>
@@ -2478,13 +2478,13 @@
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I42" t="s">
         <v>129</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="60">
@@ -2492,29 +2492,29 @@
         <v>139</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I43" t="s">
         <v>129</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="105">
@@ -2522,29 +2522,29 @@
         <v>140</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="G44"/>
       <c r="H44" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I44" t="s">
         <v>129</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="90">
@@ -2552,29 +2552,29 @@
         <v>141</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="G45"/>
       <c r="H45" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I45" t="s">
         <v>129</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="105">
@@ -2582,29 +2582,29 @@
         <v>142</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="G46"/>
       <c r="H46" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I46" t="s">
         <v>129</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45">
@@ -2931,16 +2931,16 @@
     </row>
     <row r="59" spans="1:11" ht="60">
       <c r="A59" t="s">
+        <v>233</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>235</v>
-      </c>
       <c r="C59" t="s">
         <v>14</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E59" t="s">
         <v>34</v>
@@ -2950,7 +2950,7 @@
       </c>
       <c r="G59"/>
       <c r="H59" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J59" s="6" t="s">
         <v>11</v>
@@ -2958,16 +2958,16 @@
     </row>
     <row r="60" spans="1:11" ht="105">
       <c r="A60" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E60" t="s">
         <v>34</v>
@@ -2977,24 +2977,24 @@
       </c>
       <c r="G60"/>
       <c r="H60" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="J60" s="6" t="s">
         <v>227</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="120">
       <c r="A61" t="s">
+        <v>228</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>230</v>
-      </c>
       <c r="C61" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E61" t="s">
         <v>34</v>
@@ -3004,18 +3004,18 @@
       </c>
       <c r="G61"/>
       <c r="H61" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="J61" s="6" t="s">
         <v>232</v>
-      </c>
-      <c r="J61" s="6" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="30">
       <c r="A62" t="s">
+        <v>244</v>
+      </c>
+      <c r="B62" s="12" t="s">
         <v>245</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>246</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -3030,30 +3030,30 @@
         <v>35</v>
       </c>
       <c r="G62" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="H62" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="H62" s="14" t="s">
-        <v>248</v>
-      </c>
       <c r="J62" s="6" t="s">
-        <v>249</v>
+        <v>11</v>
       </c>
       <c r="K62" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="45">
       <c r="A63" t="s">
+        <v>248</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="9" t="s">
         <v>250</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C63" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>252</v>
       </c>
       <c r="E63" t="s">
         <v>0</v>
@@ -3061,7 +3061,7 @@
       <c r="G63"/>
       <c r="H63"/>
       <c r="J63" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K63" t="s">
         <v>60</v>
@@ -3069,16 +3069,16 @@
     </row>
     <row r="64" spans="1:11" ht="30">
       <c r="A64" t="s">
+        <v>253</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="9" t="s">
         <v>255</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="C64" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>257</v>
       </c>
       <c r="E64" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Replaced bouncing mails in IAM and OAUTH testdata files
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="266">
   <si>
     <t>GET</t>
   </si>
@@ -419,8 +419,413 @@
     <t>/user</t>
   </si>
   <si>
+    <t>OPQA-2706_2</t>
+  </si>
+  <si>
+    <t>userid</t>
+  </si>
+  <si>
+    <t>X-1P-User=(OPQA-2706_2_userid)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>{"loginid":"(OPQA-542_email)","password":"1Platform"}</t>
+  </si>
+  <si>
+    <t>OPQA-3757</t>
+  </si>
+  <si>
+    <t>OPQA-3758</t>
+  </si>
+  <si>
+    <t>OPQA-3759</t>
+  </si>
+  <si>
+    <t>OPQA-3760</t>
+  </si>
+  <si>
+    <t>OPQA-3761</t>
+  </si>
+  <si>
+    <t>OPQA-3762</t>
+  </si>
+  <si>
+    <t>OPQA-3763</t>
+  </si>
+  <si>
+    <t>OPQA-3764</t>
+  </si>
+  <si>
+    <t>OPQA-3765</t>
+  </si>
+  <si>
+    <t>OPQA-3546</t>
+  </si>
+  <si>
+    <t>Verify that to register neon account with special symbol(+) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)+@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)+@sharklasers.com</t>
+  </si>
+  <si>
+    <t>OPQA-3547</t>
+  </si>
+  <si>
+    <t>Verify that to register neon account with special symbol(-) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)-@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)-@sharklasers.com</t>
+  </si>
+  <si>
+    <t>OPQA-3548</t>
+  </si>
+  <si>
+    <t>Verify that to register neon account with special symbols(.) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss).@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss).@sharklasers.com</t>
+  </si>
+  <si>
+    <t>OPQA-3549</t>
+  </si>
+  <si>
+    <t>Verify that to register neon account with special symbols( _) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)_@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)_@sharklasers.com</t>
+  </si>
+  <si>
+    <t>OPQA-3550</t>
+  </si>
+  <si>
+    <t>Verify that to register endnote account using 1P AUTH API</t>
+  </si>
+  <si>
+    <t>/account/register/endnote</t>
+  </si>
+  <si>
+    <t>OPQA-3551</t>
+  </si>
+  <si>
+    <t>Verify that to register EndNote account with special symbol(+) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>OPQA-3552</t>
+  </si>
+  <si>
+    <t>Verify that to register EndNote account with special symbol(-) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>OPQA-3553</t>
+  </si>
+  <si>
+    <t>Verify that to register EndNote account with special symbols(.) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>OPQA-3554</t>
+  </si>
+  <si>
+    <t>Verify that to register EndNote account with special symbols( _) using 1PAUTH API   </t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1+@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1-@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1.@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1_@sharklasers.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)1@sharklasers.com</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)1+@sharklasers.com</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)1-@sharklasers.com</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)1.@sharklasers.com</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)1_@sharklasers.com</t>
+  </si>
+  <si>
+    <t>OPQA-3563</t>
+  </si>
+  <si>
+    <t>Verify that to get error status when user trying get account settings by passing wrong truid</t>
+  </si>
+  <si>
+    <t>status=400</t>
+  </si>
+  <si>
+    <t>OPQA-3564</t>
+  </si>
+  <si>
+    <t>Verify that to settings api able to change primary account.</t>
+  </si>
+  <si>
+    <t>status=200||message=Successfully updated user settings||status=200</t>
+  </si>
+  <si>
+    <t>{"preferredEmailProvider":"steam","userid":"2a326b50-2f08-11e6-a908-cd1e75e72744"}</t>
+  </si>
+  <si>
+    <t>{"preferredEmailProvider":"facebook","userid":"2a326b50-2f08-11e6-a908-cd1e75e72744"}</t>
+  </si>
+  <si>
+    <t>OPQA-3564_1</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the user password by passing wrong userid using 1PAuth API</t>
+  </si>
+  <si>
+    <t>OPQA-3768</t>
+  </si>
+  <si>
+    <t>status=412||reason=Activate Registered account to continue||truid=(OPQA-2779_truid)||errorcode=412</t>
+  </si>
+  <si>
+    <t>status=200||message=Your password has been changed successfully!</t>
+  </si>
+  <si>
+    <t>status=422||reason=Password should contain at least one alphabet character, either upper or lower case</t>
+  </si>
+  <si>
+    <t>/account/auth/resetpassword</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon@123", "newpassword":"Neon_123" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"Neon_123" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"Neon@123" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"1234567890@" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"123" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"123@" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"ABCDEFG@" }</t>
+  </si>
+  <si>
+    <t>{ "password":"Neon_123", "newpassword":"ABC@" }</t>
+  </si>
+  <si>
+    <t>status=401||errorcode=401||reason=STeAM id is not found</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the user password by passing empty userid using 1PAuth API</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||reason=Invalid or empty User ID</t>
+  </si>
+  <si>
+    <t>Verify that to change user’s password  by passing valid current password and new password using 1PAuth API.</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the user password by passing wrong current password using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing current password in new password paramenter using 1PAuth API.</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing one of the previous password in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password(numeric and special character) in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing empty password in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password(combination of numbers and special characters below 8 characters) in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password(combination of alphabets and special characters) in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing invalid password(combination of alphabets and special characters below 8 characters) in newpassword parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>Verify that to get error status while changing the password by passing empty password in password parameter using 1PAuth API</t>
+  </si>
+  <si>
+    <t>{ "password":" ", "newpassword":"Neon_123" }</t>
+  </si>
+  <si>
+    <t>X-1P-User=||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>OPQA-3907</t>
+  </si>
+  <si>
+    <t>OPQA-3908</t>
+  </si>
+  <si>
+    <t>OPQA-3909</t>
+  </si>
+  <si>
+    <t>status=404||errorcode=404||reason=Incorrect password. Please try again.</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>OPQA-4609</t>
+  </si>
+  <si>
+    <t>{ "token":"1234eyJ0eXAiOiJKV1QiLCJhbGciOiJIUzI1NiJ9.eyJzdWIiOiJlMmMwM2NmOC0yZGVhLTRlOTUtYTdkYy02MmUyMmUxNzQ5Y2UiLCIxcDpwcmQiOiJzdGVhbSIsIjFwOmFwcCI6ImlwYSIsImlzcyI6IjFwIiwiMXA6ZW1sIjoiZGVjb3JhdG9yLm5lb24xQGdtYWlsLmNvbSIsImV4cCI6MTQ4MTE5MTI5OCwiaWF0IjoxNDgxMTkwMzk4LCJqdGkiOiJkMDgyYTQzYi03MjMwLTRlYjktYWExNi1kYmFkYWYzNzBmMWQifQ.6PU96_rIfMn9iqehnjotbWM9cGmvjZqPqY4NNS_JMXs" }</t>
+  </si>
+  <si>
+    <t>status=200||result=false</t>
+  </si>
+  <si>
+    <t>OPQA-4612</t>
+  </si>
+  <si>
+    <t>Verify that to get error response by passing invalid token and valid new password and app name using resetpassword API.</t>
+  </si>
+  <si>
+    <t>Verify that to get error status by passing invalid token when validating the token of user for password change using Validatetoken API.</t>
+  </si>
+  <si>
+    <t>{ "token":"123eyJ0eXAiOiJKV1QiLCJhbGciOiJIUzI1NiJ9.eyJzdWIiOiJmYzE0Yjg0MC03ZmM1LTExZTYtODBhOC0wOTUwZDBkY2IxNzciLCIxcDpwcmQiOiJzdGVhbSIsIjFwOmFwcCI6Im5lb24iLCJpc3MiOiIxcCIsIjFwOmVtbCI6ImRyYXRlc3R1c2VyMTIyMUBnbWFpbC5jb20iLCJleHAiOjE0ODExODk4MTYsImlhdCI6MTQ4MTE4ODkxNiwianRpIjoiMzJmNjk1NjItYTIzZS00ZjU3LWExM2YtNjNhNDViNmYwODZlIn0.SHqXlZwgSt2wrownV3h3pCCZ2IRyAqaPEmLMq_fQ_gg", "password":"Neon$123", "app":"Neon" }</t>
+  </si>
+  <si>
+    <t>status=404||reason=Invalid Token</t>
+  </si>
+  <si>
+    <t>OPQA-4606</t>
+  </si>
+  <si>
+    <t>Verify that to send forget password to change password by passing userid and app name parameters using forgetpassword API.</t>
+  </si>
+  <si>
+    <t>{ "loginid":"decorator.neon1@gmail.com", "app":"neon" }</t>
+  </si>
+  <si>
+    <t>/account/forgotpassword</t>
+  </si>
+  <si>
+    <t>/account/validatetoken</t>
+  </si>
+  <si>
+    <t>/account/resetpassword</t>
+  </si>
+  <si>
+    <t>status=200||steamid=394389||truid=(SYS_USER2)||loginid=project.neon2@gmail.com</t>
+  </si>
+  <si>
+    <t>x-1p-zuul-host=http://dev.1p.clarivate.com</t>
+  </si>
+  <si>
+    <t>/account/email/(SYS_USER2)a</t>
+  </si>
+  <si>
+    <t>/account/email/(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>status=404||reason=Missing/Wrong user crendentials||errorcode=404</t>
+  </si>
+  <si>
+    <t>OPQA-5579</t>
+  </si>
+  <si>
+    <t>Verify that valid short term token is able to generate using 1pAuth API</t>
+  </si>
+  <si>
+    <t>?provider=steam</t>
+  </si>
+  <si>
+    <t>{"loginid":"project.neon2@gmail.com","password":"1Platform!"}</t>
+  </si>
+  <si>
+    <t>OPQA-5580</t>
+  </si>
+  <si>
+    <t>Verify that valid long term token is generated by using short term token</t>
+  </si>
+  <si>
+    <t>/session/user/(OPQA-5579_token)</t>
+  </si>
+  <si>
+    <t>token||userid</t>
+  </si>
+  <si>
+    <t>status=200||userid=(OPQA-5579_userid)</t>
+  </si>
+  <si>
+    <t>OPQA-5581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that to get error status for  invalid long term token </t>
+  </si>
+  <si>
+    <t>/session/user/eyJ0eXAiOiJKiJ9eyJzdWIiOiIxNzRjMWF.tyyioikok</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=0||reason=New password should not match current password</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=0||reason=New password should not match previous 4 passwords</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=0||reason=Update request body is missing required parameters</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=0</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=0||reason=Password should be at least 8 characters long||reason=Password should contain at least one alphabet character, either upper or lower case</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=0||reason=Password should have at least 1 numeric character</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=0||reason=Password should be at least 8 characters long||reason=Password should have at least 1 numeric character</t>
+  </si>
+  <si>
+    <t>X-1P-User=(OPQA-2706_2_userid)||Content-Type=application/json||x-1p-zuul-host=http://localhost:7001</t>
+  </si>
+  <si>
+    <t>X-1P-User=(OPQA-2706_2_userid)1||Content-Type=application/json||x-1p-zuul-host=http://localhost:7001</t>
+  </si>
+  <si>
     <t>{
-    "userName" : "(ddMMMyyyy_HHmmss)@tr.com",
+    "userName" : "neontestuser007+(ddMMMyyyy_HHmmss)@gmail.com",
     "password" : "Neon@123",
     "firstName" : "test",
     "lastName" : "user",
@@ -428,412 +833,10 @@
 }</t>
   </si>
   <si>
-    <t>OPQA-2706_2</t>
-  </si>
-  <si>
-    <t>{"loginid":"(ddMMMyyyy_HHmmss)@tr.com","password":"Neon@123"}</t>
-  </si>
-  <si>
-    <t>userid</t>
-  </si>
-  <si>
-    <t>X-1P-User=(OPQA-2706_2_userid)||Content-Type=application/json</t>
-  </si>
-  <si>
-    <t>{"loginid":"(OPQA-542_email)","password":"1Platform"}</t>
-  </si>
-  <si>
-    <t>OPQA-3757</t>
-  </si>
-  <si>
-    <t>OPQA-3758</t>
-  </si>
-  <si>
-    <t>OPQA-3759</t>
-  </si>
-  <si>
-    <t>OPQA-3760</t>
-  </si>
-  <si>
-    <t>OPQA-3761</t>
-  </si>
-  <si>
-    <t>OPQA-3762</t>
-  </si>
-  <si>
-    <t>OPQA-3763</t>
-  </si>
-  <si>
-    <t>OPQA-3764</t>
-  </si>
-  <si>
-    <t>OPQA-3765</t>
-  </si>
-  <si>
-    <t>OPQA-3546</t>
-  </si>
-  <si>
-    <t>Verify that to register neon account with special symbol(+) using 1PAUTH API   </t>
-  </si>
-  <si>
-    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)+@sharklasers.com","password":"Neon@123"}</t>
-  </si>
-  <si>
-    <t>status=200||email=(ddMMMyyyy_HHmmss)+@sharklasers.com</t>
-  </si>
-  <si>
-    <t>OPQA-3547</t>
-  </si>
-  <si>
-    <t>Verify that to register neon account with special symbol(-) using 1PAUTH API   </t>
-  </si>
-  <si>
-    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)-@sharklasers.com","password":"Neon@123"}</t>
-  </si>
-  <si>
-    <t>status=200||email=(ddMMMyyyy_HHmmss)-@sharklasers.com</t>
-  </si>
-  <si>
-    <t>OPQA-3548</t>
-  </si>
-  <si>
-    <t>Verify that to register neon account with special symbols(.) using 1PAUTH API   </t>
-  </si>
-  <si>
-    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss).@sharklasers.com","password":"Neon@123"}</t>
-  </si>
-  <si>
-    <t>status=200||email=(ddMMMyyyy_HHmmss).@sharklasers.com</t>
-  </si>
-  <si>
-    <t>OPQA-3549</t>
-  </si>
-  <si>
-    <t>Verify that to register neon account with special symbols( _) using 1PAUTH API   </t>
-  </si>
-  <si>
-    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)_@sharklasers.com","password":"Neon@123"}</t>
-  </si>
-  <si>
-    <t>status=200||email=(ddMMMyyyy_HHmmss)_@sharklasers.com</t>
-  </si>
-  <si>
-    <t>OPQA-3550</t>
-  </si>
-  <si>
-    <t>Verify that to register endnote account using 1P AUTH API</t>
-  </si>
-  <si>
-    <t>/account/register/endnote</t>
-  </si>
-  <si>
-    <t>OPQA-3551</t>
-  </si>
-  <si>
-    <t>Verify that to register EndNote account with special symbol(+) using 1PAUTH API   </t>
-  </si>
-  <si>
-    <t>OPQA-3552</t>
-  </si>
-  <si>
-    <t>Verify that to register EndNote account with special symbol(-) using 1PAUTH API   </t>
-  </si>
-  <si>
-    <t>OPQA-3553</t>
-  </si>
-  <si>
-    <t>Verify that to register EndNote account with special symbols(.) using 1PAUTH API   </t>
-  </si>
-  <si>
-    <t>OPQA-3554</t>
-  </si>
-  <si>
-    <t>Verify that to register EndNote account with special symbols( _) using 1PAUTH API   </t>
-  </si>
-  <si>
-    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1@sharklasers.com","password":"Neon@123"}</t>
-  </si>
-  <si>
-    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1+@sharklasers.com","password":"Neon@123"}</t>
-  </si>
-  <si>
-    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1-@sharklasers.com","password":"Neon@123"}</t>
-  </si>
-  <si>
-    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1.@sharklasers.com","password":"Neon@123"}</t>
-  </si>
-  <si>
-    <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)1_@sharklasers.com","password":"Neon@123"}</t>
-  </si>
-  <si>
-    <t>status=200||email=(ddMMMyyyy_HHmmss)1@sharklasers.com</t>
-  </si>
-  <si>
-    <t>status=200||email=(ddMMMyyyy_HHmmss)1+@sharklasers.com</t>
-  </si>
-  <si>
-    <t>status=200||email=(ddMMMyyyy_HHmmss)1-@sharklasers.com</t>
-  </si>
-  <si>
-    <t>status=200||email=(ddMMMyyyy_HHmmss)1.@sharklasers.com</t>
-  </si>
-  <si>
-    <t>status=200||email=(ddMMMyyyy_HHmmss)1_@sharklasers.com</t>
-  </si>
-  <si>
-    <t>OPQA-3563</t>
-  </si>
-  <si>
-    <t>Verify that to get error status when user trying get account settings by passing wrong truid</t>
-  </si>
-  <si>
-    <t>status=400</t>
-  </si>
-  <si>
-    <t>OPQA-3564</t>
-  </si>
-  <si>
-    <t>Verify that to settings api able to change primary account.</t>
-  </si>
-  <si>
-    <t>status=200||message=Successfully updated user settings||status=200</t>
-  </si>
-  <si>
-    <t>{"preferredEmailProvider":"steam","userid":"2a326b50-2f08-11e6-a908-cd1e75e72744"}</t>
-  </si>
-  <si>
-    <t>{"preferredEmailProvider":"facebook","userid":"2a326b50-2f08-11e6-a908-cd1e75e72744"}</t>
-  </si>
-  <si>
-    <t>OPQA-3564_1</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the user password by passing wrong userid using 1PAuth API</t>
-  </si>
-  <si>
-    <t>OPQA-3768</t>
-  </si>
-  <si>
-    <t>status=412||reason=Activate Registered account to continue||truid=(OPQA-2779_truid)||errorcode=412</t>
-  </si>
-  <si>
-    <t>status=200||message=Your password has been changed successfully!</t>
-  </si>
-  <si>
-    <t>status=422||reason=Password should contain at least one alphabet character, either upper or lower case</t>
-  </si>
-  <si>
-    <t>/account/auth/resetpassword</t>
-  </si>
-  <si>
-    <t>{ "password":"Neon@123", "newpassword":"Neon_123" }</t>
-  </si>
-  <si>
-    <t>{ "password":"Neon_123", "newpassword":"Neon_123" }</t>
-  </si>
-  <si>
-    <t>{ "password":"Neon_123", "newpassword":"Neon@123" }</t>
-  </si>
-  <si>
-    <t>{ "password":"Neon_123", "newpassword":"1234567890@" }</t>
-  </si>
-  <si>
-    <t>{ "password":"Neon_123", "newpassword":"" }</t>
-  </si>
-  <si>
-    <t>{ "password":"Neon_123", "newpassword":"123" }</t>
-  </si>
-  <si>
-    <t>{ "password":"Neon_123", "newpassword":"123@" }</t>
-  </si>
-  <si>
-    <t>{ "password":"Neon_123", "newpassword":"ABCDEFG@" }</t>
-  </si>
-  <si>
-    <t>{ "password":"Neon_123", "newpassword":"ABC@" }</t>
-  </si>
-  <si>
-    <t>status=401||errorcode=401||reason=STeAM id is not found</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the user password by passing empty userid using 1PAuth API</t>
-  </si>
-  <si>
-    <t>status=400||errorcode=400||reason=Invalid or empty User ID</t>
-  </si>
-  <si>
-    <t>Verify that to change user’s password  by passing valid current password and new password using 1PAuth API.</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the user password by passing wrong current password using 1PAuth API</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing current password in new password paramenter using 1PAuth API.</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing one of the previous password in newpassword parameter using 1PAuth API</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing invalid password(numeric and special character) in newpassword parameter using 1PAuth API</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing empty password in newpassword parameter using 1PAuth API</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing invalid password in newpassword parameter using 1PAuth API</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing invalid password(combination of numbers and special characters below 8 characters) in newpassword parameter using 1PAuth API</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing invalid password(combination of alphabets and special characters) in newpassword parameter using 1PAuth API</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing invalid password(combination of alphabets and special characters below 8 characters) in newpassword parameter using 1PAuth API</t>
-  </si>
-  <si>
-    <t>Verify that to get error status while changing the password by passing empty password in password parameter using 1PAuth API</t>
-  </si>
-  <si>
-    <t>{ "password":" ", "newpassword":"Neon_123" }</t>
-  </si>
-  <si>
-    <t>X-1P-User=||Content-Type=application/json</t>
-  </si>
-  <si>
-    <t>OPQA-3907</t>
-  </si>
-  <si>
-    <t>OPQA-3908</t>
-  </si>
-  <si>
-    <t>OPQA-3909</t>
-  </si>
-  <si>
-    <t>status=404||errorcode=404||reason=Incorrect password. Please try again.</t>
-  </si>
-  <si>
-    <t>status=200||userId=(SYS_USER2)</t>
-  </si>
-  <si>
-    <t>OPQA-4609</t>
-  </si>
-  <si>
-    <t>{ "token":"1234eyJ0eXAiOiJKV1QiLCJhbGciOiJIUzI1NiJ9.eyJzdWIiOiJlMmMwM2NmOC0yZGVhLTRlOTUtYTdkYy02MmUyMmUxNzQ5Y2UiLCIxcDpwcmQiOiJzdGVhbSIsIjFwOmFwcCI6ImlwYSIsImlzcyI6IjFwIiwiMXA6ZW1sIjoiZGVjb3JhdG9yLm5lb24xQGdtYWlsLmNvbSIsImV4cCI6MTQ4MTE5MTI5OCwiaWF0IjoxNDgxMTkwMzk4LCJqdGkiOiJkMDgyYTQzYi03MjMwLTRlYjktYWExNi1kYmFkYWYzNzBmMWQifQ.6PU96_rIfMn9iqehnjotbWM9cGmvjZqPqY4NNS_JMXs" }</t>
-  </si>
-  <si>
-    <t>status=200||result=false</t>
-  </si>
-  <si>
-    <t>OPQA-4612</t>
-  </si>
-  <si>
-    <t>Verify that to get error response by passing invalid token and valid new password and app name using resetpassword API.</t>
-  </si>
-  <si>
-    <t>Verify that to get error status by passing invalid token when validating the token of user for password change using Validatetoken API.</t>
-  </si>
-  <si>
-    <t>{ "token":"123eyJ0eXAiOiJKV1QiLCJhbGciOiJIUzI1NiJ9.eyJzdWIiOiJmYzE0Yjg0MC03ZmM1LTExZTYtODBhOC0wOTUwZDBkY2IxNzciLCIxcDpwcmQiOiJzdGVhbSIsIjFwOmFwcCI6Im5lb24iLCJpc3MiOiIxcCIsIjFwOmVtbCI6ImRyYXRlc3R1c2VyMTIyMUBnbWFpbC5jb20iLCJleHAiOjE0ODExODk4MTYsImlhdCI6MTQ4MTE4ODkxNiwianRpIjoiMzJmNjk1NjItYTIzZS00ZjU3LWExM2YtNjNhNDViNmYwODZlIn0.SHqXlZwgSt2wrownV3h3pCCZ2IRyAqaPEmLMq_fQ_gg", "password":"Neon$123", "app":"Neon" }</t>
-  </si>
-  <si>
-    <t>status=404||reason=Invalid Token</t>
-  </si>
-  <si>
-    <t>OPQA-4606</t>
-  </si>
-  <si>
-    <t>Verify that to send forget password to change password by passing userid and app name parameters using forgetpassword API.</t>
-  </si>
-  <si>
-    <t>{ "loginid":"decorator.neon1@gmail.com", "app":"neon" }</t>
-  </si>
-  <si>
-    <t>/account/forgotpassword</t>
-  </si>
-  <si>
-    <t>/account/validatetoken</t>
-  </si>
-  <si>
-    <t>/account/resetpassword</t>
-  </si>
-  <si>
-    <t>status=200||steamid=394389||truid=(SYS_USER2)||loginid=project.neon2@gmail.com</t>
-  </si>
-  <si>
-    <t>x-1p-zuul-host=http://dev.1p.clarivate.com</t>
-  </si>
-  <si>
-    <t>/account/email/(SYS_USER2)a</t>
-  </si>
-  <si>
-    <t>/account/email/(SYS_USER2)</t>
-  </si>
-  <si>
-    <t>status=404||reason=Missing/Wrong user crendentials||errorcode=404</t>
-  </si>
-  <si>
-    <t>OPQA-5579</t>
-  </si>
-  <si>
-    <t>Verify that valid short term token is able to generate using 1pAuth API</t>
-  </si>
-  <si>
-    <t>?provider=steam</t>
-  </si>
-  <si>
-    <t>{"loginid":"project.neon2@gmail.com","password":"1Platform!"}</t>
-  </si>
-  <si>
-    <t>OPQA-5580</t>
-  </si>
-  <si>
-    <t>Verify that valid long term token is generated by using short term token</t>
-  </si>
-  <si>
-    <t>/session/user/(OPQA-5579_token)</t>
-  </si>
-  <si>
-    <t>token||userid</t>
-  </si>
-  <si>
-    <t>status=200||userid=(OPQA-5579_userid)</t>
-  </si>
-  <si>
-    <t>OPQA-5581</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that to get error status for  invalid long term token </t>
-  </si>
-  <si>
-    <t>/session/user/eyJ0eXAiOiJKiJ9eyJzdWIiOiIxNzRjMWF.tyyioikok</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=0||reason=New password should not match current password</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=0||reason=New password should not match previous 4 passwords</t>
-  </si>
-  <si>
-    <t>status=400||errorcode=0||reason=Update request body is missing required parameters</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=0</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=0||reason=Password should be at least 8 characters long||reason=Password should contain at least one alphabet character, either upper or lower case</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=0||reason=Password should have at least 1 numeric character</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=0||reason=Password should be at least 8 characters long||reason=Password should have at least 1 numeric character</t>
-  </si>
-  <si>
-    <t>X-1P-User=(OPQA-2706_2_userid)||Content-Type=application/json||x-1p-zuul-host=http://localhost:7001</t>
-  </si>
-  <si>
-    <t>X-1P-User=(OPQA-2706_2_userid)1||Content-Type=application/json||x-1p-zuul-host=http://localhost:7001</t>
+    <t>{"loginid":"neontestuser007+(ddMMMyyyy_HHmmss)@gmail.com","password":"Neon@123"}</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1262,7 +1265,7 @@
   <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L89"/>
+      <selection activeCell="L2" sqref="L2:L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1336,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>16</v>
@@ -1347,6 +1350,9 @@
         <v>11</v>
       </c>
       <c r="K2" s="1"/>
+      <c r="L2" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
@@ -1365,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
@@ -1496,7 +1502,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>34</v>
@@ -1525,7 +1531,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>34</v>
@@ -1551,7 +1557,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>34</v>
@@ -1676,13 +1682,13 @@
       </c>
       <c r="G14"/>
       <c r="H14" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
@@ -1707,7 +1713,7 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45">
@@ -1757,7 +1763,7 @@
         <v>71</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30">
@@ -2129,7 +2135,7 @@
         <v>116</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
@@ -2181,7 +2187,7 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="6" t="s">
-        <v>128</v>
+        <v>263</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>11</v>
@@ -2189,7 +2195,7 @@
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>65</v>
@@ -2208,7 +2214,7 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="6" t="s">
-        <v>130</v>
+        <v>264</v>
       </c>
       <c r="I33" t="s">
         <v>124</v>
@@ -2217,402 +2223,402 @@
         <v>11</v>
       </c>
       <c r="K33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="60">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G34"/>
       <c r="H34" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60">
       <c r="A35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C35" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60">
       <c r="A36" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60">
       <c r="A37" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G37"/>
       <c r="H37" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G38"/>
       <c r="H38" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="75">
       <c r="A39" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="75">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="60">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="60">
       <c r="A42" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="60">
       <c r="A43" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="105">
       <c r="A44" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G44"/>
       <c r="H44" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="90">
       <c r="A45" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G45"/>
       <c r="H45" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="105">
       <c r="A46" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G46"/>
       <c r="H46" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45">
       <c r="A47" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
@@ -2628,18 +2634,18 @@
       </c>
       <c r="G47"/>
       <c r="H47" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="45">
       <c r="A48" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
@@ -2655,18 +2661,18 @@
       </c>
       <c r="G48"/>
       <c r="H48" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="45">
       <c r="A49" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C49" t="s">
         <v>14</v>
@@ -2682,18 +2688,18 @@
       </c>
       <c r="G49"/>
       <c r="H49" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="45">
       <c r="A50" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C50" t="s">
         <v>14</v>
@@ -2709,24 +2715,24 @@
       </c>
       <c r="G50"/>
       <c r="H50" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="30">
       <c r="A51" t="s">
+        <v>157</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>161</v>
       </c>
       <c r="E51" t="s">
         <v>34</v>
@@ -2736,24 +2742,24 @@
       </c>
       <c r="G51"/>
       <c r="H51" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="45">
       <c r="A52" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C52" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E52" t="s">
         <v>34</v>
@@ -2763,24 +2769,24 @@
       </c>
       <c r="G52"/>
       <c r="H52" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="45">
       <c r="A53" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C53" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E53" t="s">
         <v>34</v>
@@ -2790,24 +2796,24 @@
       </c>
       <c r="G53"/>
       <c r="H53" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="45">
       <c r="A54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E54" t="s">
         <v>34</v>
@@ -2817,24 +2823,24 @@
       </c>
       <c r="G54"/>
       <c r="H54" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="45">
       <c r="A55" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E55" t="s">
         <v>34</v>
@@ -2844,18 +2850,18 @@
       </c>
       <c r="G55"/>
       <c r="H55" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="45">
       <c r="A56" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
@@ -2872,15 +2878,15 @@
       <c r="G56"/>
       <c r="H56"/>
       <c r="J56" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="30">
       <c r="A57" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C57" t="s">
         <v>14</v>
@@ -2896,18 +2902,18 @@
       </c>
       <c r="G57"/>
       <c r="H57" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="30">
       <c r="A58" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C58" t="s">
         <v>14</v>
@@ -2923,24 +2929,24 @@
       </c>
       <c r="G58"/>
       <c r="H58" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="60">
       <c r="A59" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B59" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="9" t="s">
         <v>234</v>
-      </c>
-      <c r="C59" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>236</v>
       </c>
       <c r="E59" t="s">
         <v>34</v>
@@ -2950,7 +2956,7 @@
       </c>
       <c r="G59"/>
       <c r="H59" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J59" s="6" t="s">
         <v>11</v>
@@ -2958,16 +2964,16 @@
     </row>
     <row r="60" spans="1:11" ht="105">
       <c r="A60" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E60" t="s">
         <v>34</v>
@@ -2977,24 +2983,24 @@
       </c>
       <c r="G60"/>
       <c r="H60" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="120">
       <c r="A61" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E61" t="s">
         <v>34</v>
@@ -3004,18 +3010,18 @@
       </c>
       <c r="G61"/>
       <c r="H61" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="30">
       <c r="A62" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -3030,30 +3036,30 @@
         <v>35</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K62" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="45">
       <c r="A63" t="s">
+        <v>246</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="9" t="s">
         <v>248</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="C63" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>250</v>
       </c>
       <c r="E63" t="s">
         <v>0</v>
@@ -3061,7 +3067,7 @@
       <c r="G63"/>
       <c r="H63"/>
       <c r="J63" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K63" t="s">
         <v>60</v>
@@ -3069,16 +3075,16 @@
     </row>
     <row r="64" spans="1:11" ht="30">
       <c r="A64" t="s">
+        <v>251</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="9" t="s">
         <v>253</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="C64" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>255</v>
       </c>
       <c r="E64" t="s">
         <v>0</v>
@@ -3086,7 +3092,7 @@
       <c r="G64"/>
       <c r="H64"/>
       <c r="J64" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified test data in IAMtestdata.xlsx file
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bg00483545\git\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="267">
   <si>
     <t>GET</t>
   </si>
@@ -206,9 +211,6 @@
     <t>status=200||result=false||loginid=(OPQA-542_email)m</t>
   </si>
   <si>
-    <t>{"loginid":"(OPQA-542_email)","password":"1Platform!"}</t>
-  </si>
-  <si>
     <t>status=200||userid=(SYS_USER2)</t>
   </si>
   <si>
@@ -395,9 +397,6 @@
     <t>/account/email/(OPQA-2779_truid)/activate</t>
   </si>
   <si>
-    <t>{"loginid":"(ddMMMyyyy_HHmmss)@sharklasers.com","password":"Neon@123"}</t>
-  </si>
-  <si>
     <t>Content-Type=application/json||host=dev-stable.1p.thomsonreuters.com</t>
   </si>
   <si>
@@ -428,9 +427,6 @@
     <t>X-1P-User=(OPQA-2706_2_userid)||Content-Type=application/json</t>
   </si>
   <si>
-    <t>{"loginid":"(OPQA-542_email)","password":"1Platform"}</t>
-  </si>
-  <si>
     <t>OPQA-3757</t>
   </si>
   <si>
@@ -768,9 +764,6 @@
   </si>
   <si>
     <t>?provider=steam</t>
-  </si>
-  <si>
-    <t>{"loginid":"project.neon2@gmail.com","password":"1Platform!"}</t>
   </si>
   <si>
     <t>OPQA-5580</t>
@@ -833,17 +826,32 @@
 }</t>
   </si>
   <si>
-    <t>{"loginid":"neontestuser007+(ddMMMyyyy_HHmmss)@gmail.com","password":"Neon@123"}</t>
-  </si>
-  <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>{"loginid":"(OPQA-542_email)","password":"1Platform!","app":"cmty"}</t>
+  </si>
+  <si>
+    <t>{"loginid":"(OPQA-542_email)","password":"1Platform","app":"cmty"}</t>
+  </si>
+  <si>
+    <t>{"loginid":"(OPQA-542_email)","password":"1Platform!""app":"cmty"}</t>
+  </si>
+  <si>
+    <t>{"loginid":"(ddMMMyyyy_HHmmss)@sharklasers.com","password":"Neon@123",app="cmty"}</t>
+  </si>
+  <si>
+    <t>{"loginid":"neontestuser007+(ddMMMyyyy_HHmmss)@gmail.com","password":"Neon@123","app":"cmty"}</t>
+  </si>
+  <si>
+    <t>{"loginid":"project.neon2@gmail.com","password":"1Platform!","app":"cmty"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -974,6 +982,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1020,7 +1036,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1052,9 +1068,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1086,6 +1103,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1261,14 +1279,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L65"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="33" style="6" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1284,7 +1302,7 @@
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1322,7 +1340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45">
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1339,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>16</v>
@@ -1351,10 +1369,10 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="45">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1371,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
@@ -1383,7 +1401,7 @@
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="30">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1412,7 +1430,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="105">
+    <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1439,7 +1457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="60">
+    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1466,7 +1484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30">
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1491,7 +1509,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="135">
+    <row r="8" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1502,7 +1520,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>34</v>
@@ -1520,7 +1538,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="135">
+    <row r="9" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1531,7 +1549,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>34</v>
@@ -1546,7 +1564,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="135">
+    <row r="10" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1557,7 +1575,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>34</v>
@@ -1578,12 +1596,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="45">
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -1603,12 +1621,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="45">
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -1628,12 +1646,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -1649,24 +1667,24 @@
       </c>
       <c r="G13"/>
       <c r="H13" s="6" t="s">
-        <v>58</v>
+        <v>261</v>
       </c>
       <c r="I13" t="s">
         <v>22</v>
       </c>
       <c r="J13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" t="s">
         <v>59</v>
       </c>
-      <c r="K13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30">
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -1682,27 +1700,27 @@
       </c>
       <c r="G14"/>
       <c r="H14" s="6" t="s">
-        <v>131</v>
+        <v>262</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>0</v>
@@ -1713,46 +1731,46 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="45">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
       <c r="J16" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="30">
-      <c r="A17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>0</v>
@@ -1760,49 +1778,49 @@
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="30">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30">
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>0</v>
@@ -1810,24 +1828,24 @@
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="45">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>21</v>
@@ -1837,18 +1855,18 @@
       </c>
       <c r="G20"/>
       <c r="H20" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30">
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
@@ -1864,27 +1882,27 @@
       </c>
       <c r="G21"/>
       <c r="H21" s="6" t="s">
-        <v>58</v>
+        <v>261</v>
       </c>
       <c r="I21" t="s">
         <v>22</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="30">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>21</v>
@@ -1894,18 +1912,18 @@
       </c>
       <c r="G22"/>
       <c r="H22" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="30">
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
@@ -1921,30 +1939,30 @@
       </c>
       <c r="G23"/>
       <c r="H23" s="6" t="s">
-        <v>58</v>
+        <v>263</v>
       </c>
       <c r="I23" t="s">
         <v>22</v>
       </c>
       <c r="J23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23" t="s">
         <v>59</v>
       </c>
-      <c r="K23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="30">
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>21</v>
@@ -1954,24 +1972,24 @@
       </c>
       <c r="G24"/>
       <c r="H24" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="45">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>100</v>
-      </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>0</v>
@@ -1979,24 +1997,24 @@
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="30">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>21</v>
@@ -2006,18 +2024,18 @@
       </c>
       <c r="G26"/>
       <c r="H26" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="60">
+    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>103</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
@@ -2033,30 +2051,30 @@
       </c>
       <c r="G27"/>
       <c r="H27" s="6" t="s">
-        <v>58</v>
+        <v>261</v>
       </c>
       <c r="I27" t="s">
         <v>22</v>
       </c>
       <c r="J27" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K27" t="s">
         <v>59</v>
       </c>
-      <c r="K27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="60">
+    </row>
+    <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>110</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>34</v>
@@ -2066,30 +2084,30 @@
       </c>
       <c r="G28"/>
       <c r="H28" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K28" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="30">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>34</v>
@@ -2099,21 +2117,21 @@
       </c>
       <c r="G29"/>
       <c r="H29" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="K29" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="K29" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="45">
+    </row>
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -2129,55 +2147,55 @@
       </c>
       <c r="G30"/>
       <c r="H30" s="6" t="s">
-        <v>120</v>
+        <v>264</v>
       </c>
       <c r="I30" t="s">
+        <v>115</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>116</v>
       </c>
-      <c r="J30" s="6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="30">
-      <c r="A31" t="s">
+      <c r="B31" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>119</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="105">
+    <row r="32" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="D32" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="C32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>34</v>
@@ -2187,18 +2205,18 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="6" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="30">
+    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
         <v>14</v>
@@ -2214,417 +2232,417 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="6" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="60">
-      <c r="A34" t="s">
-        <v>132</v>
-      </c>
       <c r="B34" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G34"/>
       <c r="H34" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="60">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C35" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I35" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="60">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="60">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G37"/>
       <c r="H37" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I37" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="60">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G38"/>
       <c r="H38" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I38" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="75">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I39" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="75">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I40" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="60">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I41" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="60">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I42" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="60">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I43" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="105">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G44"/>
       <c r="H44" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I44" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="90">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G45"/>
       <c r="H45" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I45" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="105">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G46"/>
       <c r="H46" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I46" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="45">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E47" t="s">
         <v>34</v>
@@ -2634,24 +2652,24 @@
       </c>
       <c r="G47"/>
       <c r="H47" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="J47" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="45">
-      <c r="A48" t="s">
-        <v>145</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>146</v>
-      </c>
       <c r="C48" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E48" t="s">
         <v>34</v>
@@ -2661,24 +2679,24 @@
       </c>
       <c r="G48"/>
       <c r="H48" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="J48" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="45">
-      <c r="A49" t="s">
-        <v>149</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>150</v>
-      </c>
       <c r="C49" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E49" t="s">
         <v>34</v>
@@ -2688,24 +2706,24 @@
       </c>
       <c r="G49"/>
       <c r="H49" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>150</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="J49" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="45">
-      <c r="A50" t="s">
-        <v>153</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="C50" t="s">
         <v>14</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E50" t="s">
         <v>34</v>
@@ -2715,24 +2733,24 @@
       </c>
       <c r="G50"/>
       <c r="H50" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="J50" s="6" t="s">
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="30">
-      <c r="A51" t="s">
-        <v>157</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>159</v>
       </c>
       <c r="E51" t="s">
         <v>34</v>
@@ -2742,24 +2760,24 @@
       </c>
       <c r="G51"/>
       <c r="H51" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="45">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C52" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E52" t="s">
         <v>34</v>
@@ -2769,24 +2787,24 @@
       </c>
       <c r="G52"/>
       <c r="H52" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C53" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E53" t="s">
         <v>34</v>
@@ -2796,24 +2814,24 @@
       </c>
       <c r="G53"/>
       <c r="H53" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="45">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E54" t="s">
         <v>34</v>
@@ -2823,24 +2841,24 @@
       </c>
       <c r="G54"/>
       <c r="H54" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E55" t="s">
         <v>34</v>
@@ -2850,18 +2868,18 @@
       </c>
       <c r="G55"/>
       <c r="H55" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="45">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
@@ -2873,20 +2891,20 @@
         <v>0</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G56"/>
       <c r="H56"/>
       <c r="J56" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="30">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C57" t="s">
         <v>14</v>
@@ -2902,18 +2920,18 @@
       </c>
       <c r="G57"/>
       <c r="H57" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J57" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" ht="30">
-      <c r="A58" t="s">
-        <v>186</v>
-      </c>
       <c r="B58" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C58" t="s">
         <v>14</v>
@@ -2929,24 +2947,24 @@
       </c>
       <c r="G58"/>
       <c r="H58" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="60">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>228</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="C59" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>234</v>
       </c>
       <c r="E59" t="s">
         <v>34</v>
@@ -2956,24 +2974,24 @@
       </c>
       <c r="G59"/>
       <c r="H59" s="11" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="J59" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="105">
+    <row r="60" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E60" t="s">
         <v>34</v>
@@ -2983,24 +3001,24 @@
       </c>
       <c r="G60"/>
       <c r="H60" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>223</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="J60" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="120">
-      <c r="A61" t="s">
-        <v>226</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>227</v>
-      </c>
       <c r="C61" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E61" t="s">
         <v>34</v>
@@ -3010,18 +3028,18 @@
       </c>
       <c r="G61"/>
       <c r="H61" s="6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="30">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -3036,30 +3054,30 @@
         <v>35</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>245</v>
+        <v>266</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K62" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="45">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C63" t="s">
         <v>14</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E63" t="s">
         <v>0</v>
@@ -3067,24 +3085,24 @@
       <c r="G63"/>
       <c r="H63"/>
       <c r="J63" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="K63" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="30">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C64" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E64" t="s">
         <v>0</v>
@@ -3092,7 +3110,7 @@
       <c r="G64"/>
       <c r="H64"/>
       <c r="J64" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3110,12 +3128,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified validations in IAM module
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="265">
   <si>
     <t>GET</t>
   </si>
@@ -319,9 +319,6 @@
     <t>{"truid":"(SYS_USER2)" ,"userStatus":"Activate", "comments":"Activate evicted User"}</t>
   </si>
   <si>
-    <t>status=423||reason=User is evicted||errorcode=423</t>
-  </si>
-  <si>
     <t>OPQA-544</t>
   </si>
   <si>
@@ -752,9 +749,6 @@
   </si>
   <si>
     <t>/account/email/(SYS_USER2)</t>
-  </si>
-  <si>
-    <t>status=404||reason=Missing/Wrong user crendentials||errorcode=404</t>
   </si>
   <si>
     <t>OPQA-5579</t>
@@ -826,18 +820,12 @@
 }</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>{"loginid":"(OPQA-542_email)","password":"1Platform!","app":"cmty"}</t>
   </si>
   <si>
     <t>{"loginid":"(OPQA-542_email)","password":"1Platform","app":"cmty"}</t>
   </si>
   <si>
-    <t>{"loginid":"(OPQA-542_email)","password":"1Platform!""app":"cmty"}</t>
-  </si>
-  <si>
     <t>{"loginid":"(ddMMMyyyy_HHmmss)@sharklasers.com","password":"Neon@123",app="cmty"}</t>
   </si>
   <si>
@@ -845,6 +833,12 @@
   </si>
   <si>
     <t>{"loginid":"project.neon2@gmail.com","password":"1Platform!","app":"cmty"}</t>
+  </si>
+  <si>
+    <t>status=404||error_description=Missing/Wrong user crendentials||error_code=404</t>
+  </si>
+  <si>
+    <t>status=423||error_description=User is evicted||error_code=423</t>
   </si>
 </sst>
 </file>
@@ -1282,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>16</v>
@@ -1368,9 +1362,6 @@
         <v>11</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" t="s">
-        <v>260</v>
-      </c>
     </row>
     <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1389,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
@@ -1520,7 +1511,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>34</v>
@@ -1549,7 +1540,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>34</v>
@@ -1575,7 +1566,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>34</v>
@@ -1667,7 +1658,7 @@
       </c>
       <c r="G13"/>
       <c r="H13" s="6" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="I13" t="s">
         <v>22</v>
@@ -1700,13 +1691,13 @@
       </c>
       <c r="G14"/>
       <c r="H14" s="6" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>238</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1731,7 +1722,7 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1781,7 +1772,7 @@
         <v>70</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1836,7 +1827,7 @@
     </row>
     <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>89</v>
@@ -1882,13 +1873,13 @@
       </c>
       <c r="G21"/>
       <c r="H21" s="6" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="I21" t="s">
         <v>22</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>94</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1920,7 +1911,7 @@
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>64</v>
@@ -1939,7 +1930,7 @@
       </c>
       <c r="G23"/>
       <c r="H23" s="6" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="I23" t="s">
         <v>22</v>
@@ -1953,10 +1944,10 @@
     </row>
     <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
@@ -1980,16 +1971,16 @@
     </row>
     <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>0</v>
@@ -1997,15 +1988,15 @@
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>91</v>
@@ -2032,10 +2023,10 @@
     </row>
     <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
@@ -2051,7 +2042,7 @@
       </c>
       <c r="G27"/>
       <c r="H27" s="6" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="I27" t="s">
         <v>22</v>
@@ -2065,16 +2056,16 @@
     </row>
     <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>34</v>
@@ -2084,10 +2075,10 @@
       </c>
       <c r="G28"/>
       <c r="H28" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J28" s="6" t="s">
         <v>77</v>
@@ -2098,16 +2089,16 @@
     </row>
     <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>34</v>
@@ -2117,21 +2108,21 @@
       </c>
       <c r="G29"/>
       <c r="H29" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="K29" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -2147,38 +2138,38 @@
       </c>
       <c r="G30"/>
       <c r="H30" s="6" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="I30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>11</v>
@@ -2186,16 +2177,16 @@
     </row>
     <row r="32" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="C32" t="s">
         <v>123</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>34</v>
@@ -2205,7 +2196,7 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>11</v>
@@ -2213,7 +2204,7 @@
     </row>
     <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>64</v>
@@ -2232,417 +2223,417 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="I33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G34"/>
       <c r="H34" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C35" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G37"/>
       <c r="H37" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G38"/>
       <c r="H38" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G44"/>
       <c r="H44" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G45"/>
       <c r="H45" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G46"/>
       <c r="H46" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>137</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>139</v>
-      </c>
       <c r="C47" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E47" t="s">
         <v>34</v>
@@ -2652,24 +2643,24 @@
       </c>
       <c r="G47"/>
       <c r="H47" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="J47" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>143</v>
-      </c>
       <c r="C48" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E48" t="s">
         <v>34</v>
@@ -2679,24 +2670,24 @@
       </c>
       <c r="G48"/>
       <c r="H48" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J48" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>145</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>147</v>
-      </c>
       <c r="C49" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E49" t="s">
         <v>34</v>
@@ -2706,24 +2697,24 @@
       </c>
       <c r="G49"/>
       <c r="H49" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="J49" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>149</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>151</v>
-      </c>
       <c r="C50" t="s">
         <v>14</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E50" t="s">
         <v>34</v>
@@ -2733,24 +2724,24 @@
       </c>
       <c r="G50"/>
       <c r="H50" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J50" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="C51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>156</v>
       </c>
       <c r="E51" t="s">
         <v>34</v>
@@ -2760,24 +2751,24 @@
       </c>
       <c r="G51"/>
       <c r="H51" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>156</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>158</v>
-      </c>
       <c r="C52" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E52" t="s">
         <v>34</v>
@@ -2787,24 +2778,24 @@
       </c>
       <c r="G52"/>
       <c r="H52" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>158</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>160</v>
-      </c>
       <c r="C53" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E53" t="s">
         <v>34</v>
@@ -2814,24 +2805,24 @@
       </c>
       <c r="G53"/>
       <c r="H53" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>160</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B54" s="6" t="s">
-        <v>162</v>
-      </c>
       <c r="C54" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E54" t="s">
         <v>34</v>
@@ -2841,24 +2832,24 @@
       </c>
       <c r="G54"/>
       <c r="H54" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>164</v>
-      </c>
       <c r="C55" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E55" t="s">
         <v>34</v>
@@ -2868,18 +2859,18 @@
       </c>
       <c r="G55"/>
       <c r="H55" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>174</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
@@ -2896,15 +2887,15 @@
       <c r="G56"/>
       <c r="H56"/>
       <c r="J56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>177</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="C57" t="s">
         <v>14</v>
@@ -2920,18 +2911,18 @@
       </c>
       <c r="G57"/>
       <c r="H57" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C58" t="s">
         <v>14</v>
@@ -2947,24 +2938,24 @@
       </c>
       <c r="G58"/>
       <c r="H58" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>227</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>229</v>
-      </c>
       <c r="C59" t="s">
         <v>14</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E59" t="s">
         <v>34</v>
@@ -2974,7 +2965,7 @@
       </c>
       <c r="G59"/>
       <c r="H59" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J59" s="6" t="s">
         <v>11</v>
@@ -2982,16 +2973,16 @@
     </row>
     <row r="60" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E60" t="s">
         <v>34</v>
@@ -3001,24 +2992,24 @@
       </c>
       <c r="G60"/>
       <c r="H60" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="J60" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>222</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>224</v>
-      </c>
       <c r="C61" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E61" t="s">
         <v>34</v>
@@ -3028,18 +3019,18 @@
       </c>
       <c r="G61"/>
       <c r="H61" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="J61" s="6" t="s">
         <v>226</v>
-      </c>
-      <c r="J61" s="6" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -3054,30 +3045,30 @@
         <v>35</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K62" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>240</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="9" t="s">
         <v>242</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="C63" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>244</v>
       </c>
       <c r="E63" t="s">
         <v>0</v>
@@ -3085,7 +3076,7 @@
       <c r="G63"/>
       <c r="H63"/>
       <c r="J63" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K63" t="s">
         <v>59</v>
@@ -3093,16 +3084,16 @@
     </row>
     <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>245</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="9" t="s">
         <v>247</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="C64" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>249</v>
       </c>
       <c r="E64" t="s">
         <v>0</v>
@@ -3110,7 +3101,7 @@
       <c r="G64"/>
       <c r="H64"/>
       <c r="J64" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed field in IAM test data file
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L66"/>
+    <sheetView tabSelected="1" topLeftCell="G22" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Created sanity.xml file for prod release
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -595,9 +595,6 @@
     <t>OPQA-3768</t>
   </si>
   <si>
-    <t>status=412||reason=Activate Registered account to continue||truid=(OPQA-2779_truid)||errorcode=412</t>
-  </si>
-  <si>
     <t>status=200||message=Your password has been changed successfully!</t>
   </si>
   <si>
@@ -839,6 +836,9 @@
   </si>
   <si>
     <t>status=423||error_description=User is evicted||error_code=423</t>
+  </si>
+  <si>
+    <t>status=412||error_description=Activate Registered account to continue||truid=(OPQA-2779_truid)||errorcode=412</t>
   </si>
 </sst>
 </file>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G22" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>16</v>
@@ -1380,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
@@ -1511,7 +1511,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>34</v>
@@ -1540,7 +1540,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>34</v>
@@ -1566,7 +1566,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>34</v>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="G13"/>
       <c r="H13" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I13" t="s">
         <v>22</v>
@@ -1691,13 +1691,13 @@
       </c>
       <c r="G14"/>
       <c r="H14" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1722,7 +1722,7 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1772,7 +1772,7 @@
         <v>70</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1873,13 +1873,13 @@
       </c>
       <c r="G21"/>
       <c r="H21" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I21" t="s">
         <v>22</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1930,7 +1930,7 @@
       </c>
       <c r="G23"/>
       <c r="H23" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I23" t="s">
         <v>22</v>
@@ -2042,7 +2042,7 @@
       </c>
       <c r="G27"/>
       <c r="H27" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I27" t="s">
         <v>22</v>
@@ -2138,13 +2138,13 @@
       </c>
       <c r="G30"/>
       <c r="H30" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I30" t="s">
         <v>114</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>185</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2196,7 +2196,7 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>11</v>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I33" t="s">
         <v>121</v>
@@ -2240,29 +2240,29 @@
         <v>128</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G34"/>
       <c r="H34" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I34" t="s">
         <v>125</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2276,80 +2276,80 @@
         <v>14</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I35" t="s">
         <v>125</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G37"/>
       <c r="H37" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I37" t="s">
         <v>125</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2357,29 +2357,29 @@
         <v>129</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G38"/>
       <c r="H38" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I38" t="s">
         <v>125</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2387,29 +2387,29 @@
         <v>130</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I39" t="s">
         <v>125</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2417,29 +2417,29 @@
         <v>131</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I40" t="s">
         <v>125</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2447,13 +2447,13 @@
         <v>132</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>21</v>
@@ -2463,27 +2463,27 @@
       </c>
       <c r="G41"/>
       <c r="H41" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I41" t="s">
         <v>125</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>21</v>
@@ -2493,13 +2493,13 @@
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I42" t="s">
         <v>125</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2507,29 +2507,29 @@
         <v>133</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I43" t="s">
         <v>125</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -2537,29 +2537,29 @@
         <v>134</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G44"/>
       <c r="H44" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I44" t="s">
         <v>125</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -2567,29 +2567,29 @@
         <v>135</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G45"/>
       <c r="H45" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I45" t="s">
         <v>125</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -2597,29 +2597,29 @@
         <v>136</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G46"/>
       <c r="H46" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I46" t="s">
         <v>125</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2946,16 +2946,16 @@
     </row>
     <row r="59" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>226</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>228</v>
-      </c>
       <c r="C59" t="s">
         <v>14</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E59" t="s">
         <v>34</v>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="G59"/>
       <c r="H59" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J59" s="6" t="s">
         <v>11</v>
@@ -2973,16 +2973,16 @@
     </row>
     <row r="60" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E60" t="s">
         <v>34</v>
@@ -2992,24 +2992,24 @@
       </c>
       <c r="G60"/>
       <c r="H60" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="J60" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>221</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>223</v>
-      </c>
       <c r="C61" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E61" t="s">
         <v>34</v>
@@ -3019,18 +3019,18 @@
       </c>
       <c r="G61"/>
       <c r="H61" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="J61" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="J61" s="6" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>236</v>
+      </c>
+      <c r="B62" s="12" t="s">
         <v>237</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>238</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -3045,30 +3045,30 @@
         <v>35</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K62" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>239</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="9" t="s">
         <v>241</v>
-      </c>
-      <c r="C63" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>242</v>
       </c>
       <c r="E63" t="s">
         <v>0</v>
@@ -3076,7 +3076,7 @@
       <c r="G63"/>
       <c r="H63"/>
       <c r="J63" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K63" t="s">
         <v>59</v>
@@ -3084,16 +3084,16 @@
     </row>
     <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>244</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="9" t="s">
         <v>246</v>
-      </c>
-      <c r="C64" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>247</v>
       </c>
       <c r="E64" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
fixed failed script in IAM module
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -373,12 +373,6 @@
     <t>{"firstName":"neon1","lastName":"test1","userName":"(ddMMMyyyy_HHmmss)@sharklasers.com","password":"Neon@123"}</t>
   </si>
   <si>
-    <t>status=200||email=(ddMMMyyyy_HHmmss)@sharklasers.com</t>
-  </si>
-  <si>
-    <t>truid</t>
-  </si>
-  <si>
     <t>Verify that to register neon account using API</t>
   </si>
   <si>
@@ -391,9 +385,6 @@
     <t xml:space="preserve">Verify that neon API able to send verification email </t>
   </si>
   <si>
-    <t>/account/email/(OPQA-2779_truid)/activate</t>
-  </si>
-  <si>
     <t>Content-Type=application/json||host=dev-stable.1p.thomsonreuters.com</t>
   </si>
   <si>
@@ -781,25 +772,7 @@
     <t>/session/user/eyJ0eXAiOiJKiJ9eyJzdWIiOiIxNzRjMWF.tyyioikok</t>
   </si>
   <si>
-    <t>status=422||errorcode=0||reason=New password should not match current password</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=0||reason=New password should not match previous 4 passwords</t>
-  </si>
-  <si>
     <t>status=400||errorcode=0||reason=Update request body is missing required parameters</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=0</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=0||reason=Password should be at least 8 characters long||reason=Password should contain at least one alphabet character, either upper or lower case</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=0||reason=Password should have at least 1 numeric character</t>
-  </si>
-  <si>
-    <t>status=422||errorcode=0||reason=Password should be at least 8 characters long||reason=Password should have at least 1 numeric character</t>
   </si>
   <si>
     <t>X-1P-User=(OPQA-2706_2_userid)||Content-Type=application/json||x-1p-zuul-host=http://localhost:7001</t>
@@ -838,7 +811,34 @@
     <t>status=423||error_description=User is evicted||error_code=423</t>
   </si>
   <si>
-    <t>status=412||error_description=Activate Registered account to continue||truid=(OPQA-2779_truid)||errorcode=412</t>
+    <t>status=422||errorcode=422||reason=New password should not match current password</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=422</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=422||reason=Password should be at least 8 characters long||reason=Password should contain at least one alphabet character, either upper or lower case</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=422||reason=Password should have at least 1 numeric character</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=422||reason=Password should be at least 8 characters long||reason=Password should have at least 1 numeric character</t>
+  </si>
+  <si>
+    <t>status=422||errorcode=422||reason=New password should not match previous 4 passwords</t>
+  </si>
+  <si>
+    <t>status=400||errorcode=400||reason=Update request body is missing required parameters</t>
+  </si>
+  <si>
+    <t>status=200||email=(ddMMMyyyy_HHmmss)@sharklasers.com</t>
+  </si>
+  <si>
+    <t>status=412||error_description=Activate Registered account to continue||truid=(OPQA-2779_userid)||errorcode=412</t>
+  </si>
+  <si>
+    <t>/account/email/(OPQA-2779_userid)/activate</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1277,7 @@
   <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="L2" sqref="L2:L68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>16</v>
@@ -1380,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>17</v>
@@ -1511,7 +1511,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>34</v>
@@ -1540,7 +1540,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>34</v>
@@ -1566,7 +1566,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>34</v>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="G13"/>
       <c r="H13" s="6" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="I13" t="s">
         <v>22</v>
@@ -1691,13 +1691,13 @@
       </c>
       <c r="G14"/>
       <c r="H14" s="6" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="I14" t="s">
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1722,7 +1722,7 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="J15" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1772,7 +1772,7 @@
         <v>70</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1873,13 +1873,13 @@
       </c>
       <c r="G21"/>
       <c r="H21" s="6" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="I21" t="s">
         <v>22</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1930,7 +1930,7 @@
       </c>
       <c r="G23"/>
       <c r="H23" s="6" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="I23" t="s">
         <v>22</v>
@@ -2042,7 +2042,7 @@
       </c>
       <c r="G27"/>
       <c r="H27" s="6" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="I27" t="s">
         <v>22</v>
@@ -2089,10 +2089,10 @@
     </row>
     <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
@@ -2111,18 +2111,18 @@
         <v>110</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>111</v>
+        <v>262</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -2138,38 +2138,38 @@
       </c>
       <c r="G30"/>
       <c r="H30" s="6" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="I30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C31" t="s">
         <v>14</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>117</v>
+        <v>264</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>11</v>
@@ -2177,16 +2177,16 @@
     </row>
     <row r="32" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>34</v>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="G32"/>
       <c r="H32" s="6" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>11</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>64</v>
@@ -2223,411 +2223,411 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="6" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="I33" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K33" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C34" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="G34"/>
       <c r="H34" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I34" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="9" t="s">
         <v>184</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>187</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I35" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="G37"/>
       <c r="H37" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I37" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="G38"/>
       <c r="H38" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I38" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I39" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I40" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G41"/>
       <c r="H41" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G42"/>
       <c r="H42" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I42" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="G43"/>
       <c r="H43" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I43" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C44" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="G44"/>
       <c r="H44" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I44" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C45" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="G45"/>
       <c r="H45" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I45" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="G46"/>
       <c r="H46" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I46" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
@@ -2643,18 +2643,18 @@
       </c>
       <c r="G47"/>
       <c r="H47" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
@@ -2670,18 +2670,18 @@
       </c>
       <c r="G48"/>
       <c r="H48" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C49" t="s">
         <v>14</v>
@@ -2697,18 +2697,18 @@
       </c>
       <c r="G49"/>
       <c r="H49" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C50" t="s">
         <v>14</v>
@@ -2724,24 +2724,24 @@
       </c>
       <c r="G50"/>
       <c r="H50" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C51" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E51" t="s">
         <v>34</v>
@@ -2751,24 +2751,24 @@
       </c>
       <c r="G51"/>
       <c r="H51" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C52" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E52" t="s">
         <v>34</v>
@@ -2778,24 +2778,24 @@
       </c>
       <c r="G52"/>
       <c r="H52" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C53" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E53" t="s">
         <v>34</v>
@@ -2805,24 +2805,24 @@
       </c>
       <c r="G53"/>
       <c r="H53" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E54" t="s">
         <v>34</v>
@@ -2832,24 +2832,24 @@
       </c>
       <c r="G54"/>
       <c r="H54" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E55" t="s">
         <v>34</v>
@@ -2859,18 +2859,18 @@
       </c>
       <c r="G55"/>
       <c r="H55" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
@@ -2887,15 +2887,15 @@
       <c r="G56"/>
       <c r="H56"/>
       <c r="J56" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C57" t="s">
         <v>14</v>
@@ -2911,18 +2911,18 @@
       </c>
       <c r="G57"/>
       <c r="H57" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C58" t="s">
         <v>14</v>
@@ -2938,24 +2938,24 @@
       </c>
       <c r="G58"/>
       <c r="H58" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>223</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="C59" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>229</v>
       </c>
       <c r="E59" t="s">
         <v>34</v>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="G59"/>
       <c r="H59" s="11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="J59" s="6" t="s">
         <v>11</v>
@@ -2973,16 +2973,16 @@
     </row>
     <row r="60" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E60" t="s">
         <v>34</v>
@@ -2992,24 +2992,24 @@
       </c>
       <c r="G60"/>
       <c r="H60" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E61" t="s">
         <v>34</v>
@@ -3019,18 +3019,18 @@
       </c>
       <c r="G61"/>
       <c r="H61" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -3045,30 +3045,30 @@
         <v>35</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K62" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C63" t="s">
         <v>14</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E63" t="s">
         <v>0</v>
@@ -3076,7 +3076,7 @@
       <c r="G63"/>
       <c r="H63"/>
       <c r="J63" s="6" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="K63" t="s">
         <v>59</v>
@@ -3084,16 +3084,16 @@
     </row>
     <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C64" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E64" t="s">
         <v>0</v>
@@ -3101,7 +3101,7 @@
       <c r="G64"/>
       <c r="H64"/>
       <c r="J64" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed env for steam and fixed script in Iam testdata file
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -796,9 +796,6 @@
     <t>{"loginid":"(OPQA-542_email)","password":"1Platform","app":"cmty"}</t>
   </si>
   <si>
-    <t>{"loginid":"(ddMMMyyyy_HHmmss)@sharklasers.com","password":"Neon@123",app="cmty"}</t>
-  </si>
-  <si>
     <t>{"loginid":"neontestuser007+(ddMMMyyyy_HHmmss)@gmail.com","password":"Neon@123","app":"cmty"}</t>
   </si>
   <si>
@@ -839,6 +836,9 @@
   </si>
   <si>
     <t>/account/email/(OPQA-2779_userid)/activate</t>
+  </si>
+  <si>
+    <t>{"loginid":"(ddMMMyyyy_HHmmss)@sharklasers.com","password":"Neon@123","app":"cmty"}</t>
   </si>
 </sst>
 </file>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L68"/>
+    <sheetView tabSelected="1" topLeftCell="H67" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,7 +1697,7 @@
         <v>22</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1879,7 +1879,7 @@
         <v>22</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2111,7 +2111,7 @@
         <v>110</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K29" s="6" t="s">
         <v>123</v>
@@ -2138,13 +2138,13 @@
       </c>
       <c r="G30"/>
       <c r="H30" s="6" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="I30" t="s">
         <v>112</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
         <v>14</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>34</v>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="G33"/>
       <c r="H33" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I33" t="s">
         <v>118</v>
@@ -2379,7 +2379,7 @@
         <v>122</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2409,7 +2409,7 @@
         <v>122</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2469,7 +2469,7 @@
         <v>122</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
         <v>122</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -2559,7 +2559,7 @@
         <v>122</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -2589,7 +2589,7 @@
         <v>122</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -2619,7 +2619,7 @@
         <v>122</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3048,7 +3048,7 @@
         <v>235</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
validations are updated for IAM module
</commit_message>
<xml_diff>
--- a/src/test/test-data/IAMTestData.xlsx
+++ b/src/test/test-data/IAMTestData.xlsx
@@ -832,13 +832,13 @@
     <t>status=200||email=(ddMMMyyyy_HHmmss)@sharklasers.com</t>
   </si>
   <si>
-    <t>status=412||error_description=Activate Registered account to continue||truid=(OPQA-2779_userid)||errorcode=412</t>
-  </si>
-  <si>
     <t>/account/email/(OPQA-2779_userid)/activate</t>
   </si>
   <si>
     <t>{"loginid":"(ddMMMyyyy_HHmmss)@sharklasers.com","password":"Neon@123","app":"cmty"}</t>
+  </si>
+  <si>
+    <t>status=412||error_description=Activate Registered account to continue||truid=(OPQA-2779_userid)||error_code=412</t>
   </si>
 </sst>
 </file>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H67" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L72"/>
+    <sheetView tabSelected="1" topLeftCell="H25" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,13 +2138,13 @@
       </c>
       <c r="G30"/>
       <c r="H30" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I30" t="s">
         <v>112</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
         <v>14</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>34</v>

</xml_diff>